<commit_message>
unprotect sheet 1 in AAUP template
</commit_message>
<xml_diff>
--- a/data/imports/aaup-export.xlsx
+++ b/data/imports/aaup-export.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23540" windowHeight="14740"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23540" windowHeight="14740" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -4387,14 +4387,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="65" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="53" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="55" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -4412,42 +4413,14 @@
     <xf numFmtId="0" fontId="27" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="53" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="56" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4461,20 +4434,32 @@
     <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="56" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4499,6 +4484,21 @@
     </xf>
     <xf numFmtId="49" fontId="8" fillId="3" borderId="75" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -5140,7 +5140,7 @@
   </sheetPr>
   <dimension ref="A1:S50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -6983,8 +6983,8 @@
   </sheetPr>
   <dimension ref="A1:AMK8036"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7007,18 +7007,18 @@
   <sheetData>
     <row r="1" spans="1:23" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="23"/>
-      <c r="B1" s="403" t="s">
+      <c r="B1" s="395" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="403"/>
-      <c r="D1" s="403"/>
-      <c r="E1" s="403"/>
-      <c r="F1" s="403"/>
-      <c r="G1" s="403"/>
-      <c r="H1" s="403"/>
-      <c r="I1" s="403"/>
-      <c r="J1" s="403"/>
-      <c r="K1" s="403"/>
+      <c r="C1" s="395"/>
+      <c r="D1" s="395"/>
+      <c r="E1" s="395"/>
+      <c r="F1" s="395"/>
+      <c r="G1" s="395"/>
+      <c r="H1" s="395"/>
+      <c r="I1" s="395"/>
+      <c r="J1" s="395"/>
+      <c r="K1" s="395"/>
       <c r="L1" s="6" t="s">
         <v>1</v>
       </c>
@@ -7036,15 +7036,15 @@
       </c>
     </row>
     <row r="2" spans="1:23" ht="23.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="404" t="s">
+      <c r="A2" s="396" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="404"/>
-      <c r="C2" s="404"/>
-      <c r="D2" s="404"/>
-      <c r="E2" s="404"/>
-      <c r="F2" s="404"/>
-      <c r="G2" s="404"/>
+      <c r="B2" s="396"/>
+      <c r="C2" s="396"/>
+      <c r="D2" s="396"/>
+      <c r="E2" s="396"/>
+      <c r="F2" s="396"/>
+      <c r="G2" s="396"/>
       <c r="H2" s="24"/>
       <c r="I2" s="24"/>
       <c r="J2" s="24"/>
@@ -7100,13 +7100,13 @@
       <c r="B5" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="405" t="s">
+      <c r="C5" s="397" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="405"/>
-      <c r="E5" s="405"/>
-      <c r="F5" s="405"/>
-      <c r="G5" s="405"/>
+      <c r="D5" s="397"/>
+      <c r="E5" s="397"/>
+      <c r="F5" s="397"/>
+      <c r="G5" s="397"/>
       <c r="H5" s="28"/>
       <c r="I5" s="28"/>
       <c r="J5" s="28"/>
@@ -8341,18 +8341,18 @@
       <c r="P61" s="6"/>
     </row>
     <row r="62" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="395" t="s">
+      <c r="A62" s="403" t="s">
         <v>86</v>
       </c>
-      <c r="B62" s="395"/>
-      <c r="C62" s="395"/>
-      <c r="D62" s="395"/>
-      <c r="E62" s="395"/>
-      <c r="F62" s="395"/>
-      <c r="G62" s="395"/>
-      <c r="H62" s="395"/>
-      <c r="I62" s="395"/>
-      <c r="J62" s="395"/>
+      <c r="B62" s="403"/>
+      <c r="C62" s="403"/>
+      <c r="D62" s="403"/>
+      <c r="E62" s="403"/>
+      <c r="F62" s="403"/>
+      <c r="G62" s="403"/>
+      <c r="H62" s="403"/>
+      <c r="I62" s="403"/>
+      <c r="J62" s="403"/>
       <c r="K62" s="6"/>
       <c r="L62" s="6"/>
       <c r="M62" s="6"/>
@@ -8361,18 +8361,18 @@
       <c r="P62" s="6"/>
     </row>
     <row r="63" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="397" t="s">
+      <c r="A63" s="405" t="s">
         <v>87</v>
       </c>
-      <c r="B63" s="397"/>
-      <c r="C63" s="397"/>
-      <c r="D63" s="397"/>
-      <c r="E63" s="397"/>
-      <c r="F63" s="397"/>
-      <c r="G63" s="397"/>
-      <c r="H63" s="397"/>
-      <c r="I63" s="397"/>
-      <c r="J63" s="397"/>
+      <c r="B63" s="405"/>
+      <c r="C63" s="405"/>
+      <c r="D63" s="405"/>
+      <c r="E63" s="405"/>
+      <c r="F63" s="405"/>
+      <c r="G63" s="405"/>
+      <c r="H63" s="405"/>
+      <c r="I63" s="405"/>
+      <c r="J63" s="405"/>
       <c r="K63" s="6"/>
       <c r="L63" s="6"/>
       <c r="M63" s="6"/>
@@ -8381,18 +8381,18 @@
       <c r="P63" s="6"/>
     </row>
     <row r="64" spans="1:16" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="395" t="s">
+      <c r="A64" s="403" t="s">
         <v>88</v>
       </c>
-      <c r="B64" s="395"/>
-      <c r="C64" s="395"/>
-      <c r="D64" s="395"/>
-      <c r="E64" s="395"/>
-      <c r="F64" s="395"/>
-      <c r="G64" s="395"/>
-      <c r="H64" s="395"/>
-      <c r="I64" s="395"/>
-      <c r="J64" s="395"/>
+      <c r="B64" s="403"/>
+      <c r="C64" s="403"/>
+      <c r="D64" s="403"/>
+      <c r="E64" s="403"/>
+      <c r="F64" s="403"/>
+      <c r="G64" s="403"/>
+      <c r="H64" s="403"/>
+      <c r="I64" s="403"/>
+      <c r="J64" s="403"/>
       <c r="K64" s="6"/>
       <c r="L64" s="6"/>
       <c r="M64" s="6"/>
@@ -8401,18 +8401,18 @@
       <c r="P64" s="6"/>
     </row>
     <row r="65" spans="1:19" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="395" t="s">
+      <c r="A65" s="403" t="s">
         <v>89</v>
       </c>
-      <c r="B65" s="395"/>
-      <c r="C65" s="395"/>
-      <c r="D65" s="395"/>
-      <c r="E65" s="395"/>
-      <c r="F65" s="395"/>
-      <c r="G65" s="395"/>
-      <c r="H65" s="395"/>
-      <c r="I65" s="395"/>
-      <c r="J65" s="395"/>
+      <c r="B65" s="403"/>
+      <c r="C65" s="403"/>
+      <c r="D65" s="403"/>
+      <c r="E65" s="403"/>
+      <c r="F65" s="403"/>
+      <c r="G65" s="403"/>
+      <c r="H65" s="403"/>
+      <c r="I65" s="403"/>
+      <c r="J65" s="403"/>
       <c r="K65" s="6"/>
       <c r="L65" s="6"/>
       <c r="M65" s="6"/>
@@ -8421,18 +8421,18 @@
       <c r="P65" s="6"/>
     </row>
     <row r="66" spans="1:19" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="395" t="s">
+      <c r="A66" s="403" t="s">
         <v>90</v>
       </c>
-      <c r="B66" s="395"/>
-      <c r="C66" s="395"/>
-      <c r="D66" s="395"/>
-      <c r="E66" s="395"/>
-      <c r="F66" s="395"/>
-      <c r="G66" s="395"/>
-      <c r="H66" s="395"/>
-      <c r="I66" s="395"/>
-      <c r="J66" s="395"/>
+      <c r="B66" s="403"/>
+      <c r="C66" s="403"/>
+      <c r="D66" s="403"/>
+      <c r="E66" s="403"/>
+      <c r="F66" s="403"/>
+      <c r="G66" s="403"/>
+      <c r="H66" s="403"/>
+      <c r="I66" s="403"/>
+      <c r="J66" s="403"/>
       <c r="K66" s="6"/>
       <c r="L66" s="6"/>
       <c r="M66" s="6"/>
@@ -8441,18 +8441,18 @@
       <c r="P66" s="6"/>
     </row>
     <row r="67" spans="1:19" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="395" t="s">
+      <c r="A67" s="403" t="s">
         <v>91</v>
       </c>
-      <c r="B67" s="395"/>
-      <c r="C67" s="395"/>
-      <c r="D67" s="395"/>
-      <c r="E67" s="395"/>
-      <c r="F67" s="395"/>
-      <c r="G67" s="395"/>
-      <c r="H67" s="395"/>
-      <c r="I67" s="395"/>
-      <c r="J67" s="395"/>
+      <c r="B67" s="403"/>
+      <c r="C67" s="403"/>
+      <c r="D67" s="403"/>
+      <c r="E67" s="403"/>
+      <c r="F67" s="403"/>
+      <c r="G67" s="403"/>
+      <c r="H67" s="403"/>
+      <c r="I67" s="403"/>
+      <c r="J67" s="403"/>
       <c r="K67" s="6"/>
       <c r="L67" s="6"/>
       <c r="M67" s="6"/>
@@ -8461,18 +8461,18 @@
       <c r="P67" s="6"/>
     </row>
     <row r="68" spans="1:19" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="395" t="s">
+      <c r="A68" s="403" t="s">
         <v>92</v>
       </c>
-      <c r="B68" s="395"/>
-      <c r="C68" s="395"/>
-      <c r="D68" s="395"/>
-      <c r="E68" s="395"/>
-      <c r="F68" s="395"/>
-      <c r="G68" s="395"/>
-      <c r="H68" s="395"/>
-      <c r="I68" s="395"/>
-      <c r="J68" s="395"/>
+      <c r="B68" s="403"/>
+      <c r="C68" s="403"/>
+      <c r="D68" s="403"/>
+      <c r="E68" s="403"/>
+      <c r="F68" s="403"/>
+      <c r="G68" s="403"/>
+      <c r="H68" s="403"/>
+      <c r="I68" s="403"/>
+      <c r="J68" s="403"/>
       <c r="K68" s="6"/>
       <c r="L68" s="6"/>
       <c r="M68" s="6"/>
@@ -8481,18 +8481,18 @@
       <c r="P68" s="6"/>
     </row>
     <row r="69" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="396" t="s">
+      <c r="A69" s="404" t="s">
         <v>93</v>
       </c>
-      <c r="B69" s="396"/>
-      <c r="C69" s="396"/>
-      <c r="D69" s="396"/>
-      <c r="E69" s="396"/>
-      <c r="F69" s="396"/>
-      <c r="G69" s="396"/>
-      <c r="H69" s="396"/>
-      <c r="I69" s="396"/>
-      <c r="J69" s="396"/>
+      <c r="B69" s="404"/>
+      <c r="C69" s="404"/>
+      <c r="D69" s="404"/>
+      <c r="E69" s="404"/>
+      <c r="F69" s="404"/>
+      <c r="G69" s="404"/>
+      <c r="H69" s="404"/>
+      <c r="I69" s="404"/>
+      <c r="J69" s="404"/>
       <c r="K69" s="6"/>
       <c r="L69" s="6"/>
       <c r="M69" s="6"/>
@@ -16440,18 +16440,8 @@
     <row r="8035" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="8036" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="U0skjfhaB6r2xl9Bir8A4H4VDiSsSyNPC9tQJk+pMm4OA8PbnKNy5WLYEYYfaEf+bvrCkufzrh0sJFrfAt5uzQ==" saltValue="GOsggLWYQy0AJRcxdDOHtg==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="18">
-    <mergeCell ref="B1:K1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="A11:K11"/>
-    <mergeCell ref="A57:K57"/>
-    <mergeCell ref="A58:K58"/>
-    <mergeCell ref="A61:J61"/>
     <mergeCell ref="A67:J67"/>
     <mergeCell ref="A68:J68"/>
     <mergeCell ref="A69:J69"/>
@@ -16460,6 +16450,16 @@
     <mergeCell ref="A64:J64"/>
     <mergeCell ref="A65:J65"/>
     <mergeCell ref="A66:J66"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="A11:K11"/>
+    <mergeCell ref="A57:K57"/>
+    <mergeCell ref="A58:K58"/>
+    <mergeCell ref="A61:J61"/>
+    <mergeCell ref="B1:K1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C7:F7"/>
   </mergeCells>
   <dataValidations count="15">
     <dataValidation type="list" prompt="Choose from the list." sqref="C15">
@@ -16616,18 +16616,18 @@
   <sheetData>
     <row r="1" spans="1:25" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="23"/>
-      <c r="B1" s="403" t="s">
+      <c r="B1" s="395" t="s">
         <v>128</v>
       </c>
-      <c r="C1" s="403"/>
-      <c r="D1" s="403"/>
-      <c r="E1" s="403"/>
-      <c r="F1" s="403"/>
-      <c r="G1" s="403"/>
-      <c r="H1" s="403"/>
-      <c r="I1" s="403"/>
-      <c r="J1" s="403"/>
-      <c r="K1" s="403"/>
+      <c r="C1" s="395"/>
+      <c r="D1" s="395"/>
+      <c r="E1" s="395"/>
+      <c r="F1" s="395"/>
+      <c r="G1" s="395"/>
+      <c r="H1" s="395"/>
+      <c r="I1" s="395"/>
+      <c r="J1" s="395"/>
+      <c r="K1" s="395"/>
       <c r="L1" s="6" t="s">
         <v>1</v>
       </c>
@@ -16651,19 +16651,19 @@
       </c>
     </row>
     <row r="2" spans="1:25" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="415" t="s">
+      <c r="A2" s="406" t="s">
         <v>129</v>
       </c>
-      <c r="B2" s="415"/>
-      <c r="C2" s="415"/>
-      <c r="D2" s="415"/>
-      <c r="E2" s="415"/>
-      <c r="F2" s="415"/>
-      <c r="G2" s="415"/>
-      <c r="H2" s="415"/>
-      <c r="I2" s="415"/>
-      <c r="J2" s="415"/>
-      <c r="K2" s="415"/>
+      <c r="B2" s="406"/>
+      <c r="C2" s="406"/>
+      <c r="D2" s="406"/>
+      <c r="E2" s="406"/>
+      <c r="F2" s="406"/>
+      <c r="G2" s="406"/>
+      <c r="H2" s="406"/>
+      <c r="I2" s="406"/>
+      <c r="J2" s="406"/>
+      <c r="K2" s="406"/>
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
       <c r="N2" s="6"/>
@@ -16672,20 +16672,20 @@
     </row>
     <row r="3" spans="1:25" s="76" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="75"/>
-      <c r="B3" s="416" t="s">
+      <c r="B3" s="407" t="s">
         <v>130</v>
       </c>
-      <c r="C3" s="416"/>
-      <c r="D3" s="416"/>
-      <c r="E3" s="416"/>
-      <c r="F3" s="416"/>
-      <c r="G3" s="417" t="s">
+      <c r="C3" s="407"/>
+      <c r="D3" s="407"/>
+      <c r="E3" s="407"/>
+      <c r="F3" s="407"/>
+      <c r="G3" s="408" t="s">
         <v>131</v>
       </c>
-      <c r="H3" s="417"/>
-      <c r="I3" s="417"/>
-      <c r="J3" s="417"/>
-      <c r="K3" s="417"/>
+      <c r="H3" s="408"/>
+      <c r="I3" s="408"/>
+      <c r="J3" s="408"/>
+      <c r="K3" s="408"/>
       <c r="L3" s="6"/>
       <c r="M3" s="6"/>
       <c r="N3" s="6"/>
@@ -17620,17 +17620,17 @@
       <c r="R30" s="7"/>
     </row>
     <row r="31" spans="1:25" s="61" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="418"/>
-      <c r="B31" s="418"/>
-      <c r="C31" s="418"/>
-      <c r="D31" s="418"/>
-      <c r="E31" s="418"/>
-      <c r="F31" s="418"/>
-      <c r="G31" s="418"/>
-      <c r="H31" s="418"/>
-      <c r="I31" s="418"/>
-      <c r="J31" s="418"/>
-      <c r="K31" s="418"/>
+      <c r="A31" s="409"/>
+      <c r="B31" s="409"/>
+      <c r="C31" s="409"/>
+      <c r="D31" s="409"/>
+      <c r="E31" s="409"/>
+      <c r="F31" s="409"/>
+      <c r="G31" s="409"/>
+      <c r="H31" s="409"/>
+      <c r="I31" s="409"/>
+      <c r="J31" s="409"/>
+      <c r="K31" s="409"/>
       <c r="L31" s="6"/>
       <c r="M31" s="6"/>
       <c r="N31" s="6"/>
@@ -17718,19 +17718,19 @@
       <c r="R35" s="7"/>
     </row>
     <row r="36" spans="1:18" ht="69" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="412" t="s">
+      <c r="A36" s="410" t="s">
         <v>151</v>
       </c>
-      <c r="B36" s="412"/>
-      <c r="C36" s="412"/>
-      <c r="D36" s="412"/>
-      <c r="E36" s="412"/>
-      <c r="F36" s="412"/>
-      <c r="G36" s="412"/>
-      <c r="H36" s="412"/>
-      <c r="I36" s="412"/>
-      <c r="J36" s="412"/>
-      <c r="K36" s="412"/>
+      <c r="B36" s="410"/>
+      <c r="C36" s="410"/>
+      <c r="D36" s="410"/>
+      <c r="E36" s="410"/>
+      <c r="F36" s="410"/>
+      <c r="G36" s="410"/>
+      <c r="H36" s="410"/>
+      <c r="I36" s="410"/>
+      <c r="J36" s="410"/>
+      <c r="K36" s="410"/>
       <c r="L36" s="6"/>
       <c r="M36" s="6"/>
       <c r="N36" s="6"/>
@@ -17738,19 +17738,19 @@
       <c r="R36" s="7"/>
     </row>
     <row r="37" spans="1:18" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="412" t="s">
+      <c r="A37" s="410" t="s">
         <v>152</v>
       </c>
-      <c r="B37" s="412"/>
-      <c r="C37" s="412"/>
-      <c r="D37" s="412"/>
-      <c r="E37" s="412"/>
-      <c r="F37" s="412"/>
-      <c r="G37" s="412"/>
-      <c r="H37" s="412"/>
-      <c r="I37" s="412"/>
-      <c r="J37" s="412"/>
-      <c r="K37" s="412"/>
+      <c r="B37" s="410"/>
+      <c r="C37" s="410"/>
+      <c r="D37" s="410"/>
+      <c r="E37" s="410"/>
+      <c r="F37" s="410"/>
+      <c r="G37" s="410"/>
+      <c r="H37" s="410"/>
+      <c r="I37" s="410"/>
+      <c r="J37" s="410"/>
+      <c r="K37" s="410"/>
       <c r="L37" s="6"/>
       <c r="M37" s="6"/>
       <c r="N37" s="6"/>
@@ -17796,55 +17796,55 @@
       <c r="N39" s="6"/>
     </row>
     <row r="40" spans="1:18" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="414" t="s">
+      <c r="A40" s="412" t="s">
         <v>155</v>
       </c>
-      <c r="B40" s="414"/>
-      <c r="C40" s="414"/>
-      <c r="D40" s="414"/>
-      <c r="E40" s="414"/>
-      <c r="F40" s="414"/>
-      <c r="G40" s="414"/>
-      <c r="H40" s="414"/>
-      <c r="I40" s="414"/>
-      <c r="J40" s="414"/>
-      <c r="K40" s="414"/>
+      <c r="B40" s="412"/>
+      <c r="C40" s="412"/>
+      <c r="D40" s="412"/>
+      <c r="E40" s="412"/>
+      <c r="F40" s="412"/>
+      <c r="G40" s="412"/>
+      <c r="H40" s="412"/>
+      <c r="I40" s="412"/>
+      <c r="J40" s="412"/>
+      <c r="K40" s="412"/>
       <c r="L40" s="6"/>
       <c r="M40" s="6"/>
       <c r="N40" s="6"/>
     </row>
     <row r="41" spans="1:18" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="410" t="s">
+      <c r="A41" s="413" t="s">
         <v>156</v>
       </c>
-      <c r="B41" s="410"/>
-      <c r="C41" s="410"/>
-      <c r="D41" s="410"/>
-      <c r="E41" s="410"/>
-      <c r="F41" s="410"/>
-      <c r="G41" s="410"/>
-      <c r="H41" s="410"/>
-      <c r="I41" s="410"/>
-      <c r="J41" s="410"/>
-      <c r="K41" s="410"/>
+      <c r="B41" s="413"/>
+      <c r="C41" s="413"/>
+      <c r="D41" s="413"/>
+      <c r="E41" s="413"/>
+      <c r="F41" s="413"/>
+      <c r="G41" s="413"/>
+      <c r="H41" s="413"/>
+      <c r="I41" s="413"/>
+      <c r="J41" s="413"/>
+      <c r="K41" s="413"/>
       <c r="L41" s="6"/>
       <c r="M41" s="6"/>
       <c r="N41" s="6"/>
     </row>
     <row r="42" spans="1:18" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="410" t="s">
+      <c r="A42" s="413" t="s">
         <v>157</v>
       </c>
-      <c r="B42" s="410"/>
-      <c r="C42" s="410"/>
-      <c r="D42" s="410"/>
-      <c r="E42" s="410"/>
-      <c r="F42" s="410"/>
-      <c r="G42" s="410"/>
-      <c r="H42" s="410"/>
-      <c r="I42" s="410"/>
-      <c r="J42" s="410"/>
-      <c r="K42" s="410"/>
+      <c r="B42" s="413"/>
+      <c r="C42" s="413"/>
+      <c r="D42" s="413"/>
+      <c r="E42" s="413"/>
+      <c r="F42" s="413"/>
+      <c r="G42" s="413"/>
+      <c r="H42" s="413"/>
+      <c r="I42" s="413"/>
+      <c r="J42" s="413"/>
+      <c r="K42" s="413"/>
       <c r="L42" s="6"/>
       <c r="M42" s="6"/>
       <c r="N42" s="6"/>
@@ -17868,19 +17868,19 @@
       <c r="N43" s="6"/>
     </row>
     <row r="44" spans="1:18" ht="126.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="412" t="s">
+      <c r="A44" s="410" t="s">
         <v>159</v>
       </c>
-      <c r="B44" s="412"/>
-      <c r="C44" s="412"/>
-      <c r="D44" s="412"/>
-      <c r="E44" s="412"/>
-      <c r="F44" s="412"/>
-      <c r="G44" s="412"/>
-      <c r="H44" s="412"/>
-      <c r="I44" s="412"/>
-      <c r="J44" s="412"/>
-      <c r="K44" s="412"/>
+      <c r="B44" s="410"/>
+      <c r="C44" s="410"/>
+      <c r="D44" s="410"/>
+      <c r="E44" s="410"/>
+      <c r="F44" s="410"/>
+      <c r="G44" s="410"/>
+      <c r="H44" s="410"/>
+      <c r="I44" s="410"/>
+      <c r="J44" s="410"/>
+      <c r="K44" s="410"/>
       <c r="L44" s="6"/>
       <c r="M44" s="6"/>
       <c r="N44" s="6"/>
@@ -17920,11 +17920,11 @@
       <c r="N46" s="6"/>
     </row>
     <row r="47" spans="1:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="413" t="s">
+      <c r="A47" s="414" t="s">
         <v>161</v>
       </c>
-      <c r="B47" s="413"/>
-      <c r="C47" s="413"/>
+      <c r="B47" s="414"/>
+      <c r="C47" s="414"/>
       <c r="D47" s="109" t="s">
         <v>162</v>
       </c>
@@ -17942,11 +17942,11 @@
       <c r="N47" s="6"/>
     </row>
     <row r="48" spans="1:18" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="408" t="s">
+      <c r="A48" s="415" t="s">
         <v>164</v>
       </c>
-      <c r="B48" s="408"/>
-      <c r="C48" s="408"/>
+      <c r="B48" s="415"/>
+      <c r="C48" s="415"/>
       <c r="D48" s="110" t="s">
         <v>165</v>
       </c>
@@ -17964,11 +17964,11 @@
       <c r="N48" s="6"/>
     </row>
     <row r="49" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="407" t="s">
+      <c r="A49" s="416" t="s">
         <v>166</v>
       </c>
-      <c r="B49" s="407"/>
-      <c r="C49" s="407"/>
+      <c r="B49" s="416"/>
+      <c r="C49" s="416"/>
       <c r="D49" s="111" t="s">
         <v>167</v>
       </c>
@@ -17986,11 +17986,11 @@
       <c r="N49" s="6"/>
     </row>
     <row r="50" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="408" t="s">
+      <c r="A50" s="415" t="s">
         <v>168</v>
       </c>
-      <c r="B50" s="408"/>
-      <c r="C50" s="408"/>
+      <c r="B50" s="415"/>
+      <c r="C50" s="415"/>
       <c r="D50" s="110" t="s">
         <v>165</v>
       </c>
@@ -18008,11 +18008,11 @@
       <c r="N50" s="6"/>
     </row>
     <row r="51" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="407" t="s">
+      <c r="A51" s="416" t="s">
         <v>169</v>
       </c>
-      <c r="B51" s="407"/>
-      <c r="C51" s="407"/>
+      <c r="B51" s="416"/>
+      <c r="C51" s="416"/>
       <c r="D51" s="111" t="s">
         <v>165</v>
       </c>
@@ -18030,11 +18030,11 @@
       <c r="N51" s="6"/>
     </row>
     <row r="52" spans="1:14" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="408" t="s">
+      <c r="A52" s="415" t="s">
         <v>170</v>
       </c>
-      <c r="B52" s="408"/>
-      <c r="C52" s="408"/>
+      <c r="B52" s="415"/>
+      <c r="C52" s="415"/>
       <c r="D52" s="110" t="s">
         <v>165</v>
       </c>
@@ -18052,11 +18052,11 @@
       <c r="N52" s="6"/>
     </row>
     <row r="53" spans="1:14" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="407" t="s">
+      <c r="A53" s="416" t="s">
         <v>171</v>
       </c>
-      <c r="B53" s="407"/>
-      <c r="C53" s="407"/>
+      <c r="B53" s="416"/>
+      <c r="C53" s="416"/>
       <c r="D53" s="111" t="s">
         <v>165</v>
       </c>
@@ -18074,11 +18074,11 @@
       <c r="N53" s="6"/>
     </row>
     <row r="54" spans="1:14" ht="115.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="408" t="s">
+      <c r="A54" s="415" t="s">
         <v>172</v>
       </c>
-      <c r="B54" s="408"/>
-      <c r="C54" s="408"/>
+      <c r="B54" s="415"/>
+      <c r="C54" s="415"/>
       <c r="D54" s="110" t="s">
         <v>165</v>
       </c>
@@ -18096,11 +18096,11 @@
       <c r="N54" s="6"/>
     </row>
     <row r="55" spans="1:14" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="407" t="s">
+      <c r="A55" s="416" t="s">
         <v>173</v>
       </c>
-      <c r="B55" s="407"/>
-      <c r="C55" s="407"/>
+      <c r="B55" s="416"/>
+      <c r="C55" s="416"/>
       <c r="D55" s="111" t="s">
         <v>165</v>
       </c>
@@ -18134,55 +18134,55 @@
       <c r="N56" s="6"/>
     </row>
     <row r="57" spans="1:14" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="409" t="s">
+      <c r="A57" s="418" t="s">
         <v>174</v>
       </c>
-      <c r="B57" s="409"/>
-      <c r="C57" s="409"/>
-      <c r="D57" s="409"/>
-      <c r="E57" s="409"/>
-      <c r="F57" s="409"/>
-      <c r="G57" s="409"/>
-      <c r="H57" s="409"/>
-      <c r="I57" s="409"/>
-      <c r="J57" s="409"/>
-      <c r="K57" s="409"/>
+      <c r="B57" s="418"/>
+      <c r="C57" s="418"/>
+      <c r="D57" s="418"/>
+      <c r="E57" s="418"/>
+      <c r="F57" s="418"/>
+      <c r="G57" s="418"/>
+      <c r="H57" s="418"/>
+      <c r="I57" s="418"/>
+      <c r="J57" s="418"/>
+      <c r="K57" s="418"/>
       <c r="L57" s="6"/>
       <c r="M57" s="6"/>
       <c r="N57" s="6"/>
     </row>
     <row r="58" spans="1:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="409" t="s">
+      <c r="A58" s="418" t="s">
         <v>175</v>
       </c>
-      <c r="B58" s="409"/>
-      <c r="C58" s="409"/>
-      <c r="D58" s="409"/>
-      <c r="E58" s="409"/>
-      <c r="F58" s="409"/>
-      <c r="G58" s="409"/>
-      <c r="H58" s="409"/>
-      <c r="I58" s="409"/>
-      <c r="J58" s="409"/>
-      <c r="K58" s="409"/>
+      <c r="B58" s="418"/>
+      <c r="C58" s="418"/>
+      <c r="D58" s="418"/>
+      <c r="E58" s="418"/>
+      <c r="F58" s="418"/>
+      <c r="G58" s="418"/>
+      <c r="H58" s="418"/>
+      <c r="I58" s="418"/>
+      <c r="J58" s="418"/>
+      <c r="K58" s="418"/>
       <c r="L58" s="6"/>
       <c r="M58" s="6"/>
       <c r="N58" s="6"/>
     </row>
     <row r="59" spans="1:14" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="406" t="s">
+      <c r="A59" s="417" t="s">
         <v>176</v>
       </c>
-      <c r="B59" s="406"/>
-      <c r="C59" s="406"/>
-      <c r="D59" s="406"/>
-      <c r="E59" s="406"/>
-      <c r="F59" s="406"/>
-      <c r="G59" s="406"/>
-      <c r="H59" s="406"/>
-      <c r="I59" s="406"/>
-      <c r="J59" s="406"/>
-      <c r="K59" s="406"/>
+      <c r="B59" s="417"/>
+      <c r="C59" s="417"/>
+      <c r="D59" s="417"/>
+      <c r="E59" s="417"/>
+      <c r="F59" s="417"/>
+      <c r="G59" s="417"/>
+      <c r="H59" s="417"/>
+      <c r="I59" s="417"/>
+      <c r="J59" s="417"/>
+      <c r="K59" s="417"/>
       <c r="L59" s="6"/>
       <c r="M59" s="6"/>
       <c r="N59" s="6"/>
@@ -25309,32 +25309,32 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="26">
-    <mergeCell ref="B1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="G3:K3"/>
-    <mergeCell ref="A31:K31"/>
-    <mergeCell ref="A36:K36"/>
-    <mergeCell ref="A37:K37"/>
-    <mergeCell ref="A38:K38"/>
-    <mergeCell ref="A39:K39"/>
-    <mergeCell ref="A40:K40"/>
-    <mergeCell ref="A41:K41"/>
-    <mergeCell ref="A42:K42"/>
-    <mergeCell ref="A43:K43"/>
-    <mergeCell ref="A44:K44"/>
-    <mergeCell ref="A47:C47"/>
-    <mergeCell ref="A48:C48"/>
-    <mergeCell ref="A49:C49"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="A51:C51"/>
-    <mergeCell ref="A52:C52"/>
     <mergeCell ref="A59:K59"/>
     <mergeCell ref="A53:C53"/>
     <mergeCell ref="A54:C54"/>
     <mergeCell ref="A55:C55"/>
     <mergeCell ref="A57:K57"/>
     <mergeCell ref="A58:K58"/>
+    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="A49:C49"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="A51:C51"/>
+    <mergeCell ref="A52:C52"/>
+    <mergeCell ref="A41:K41"/>
+    <mergeCell ref="A42:K42"/>
+    <mergeCell ref="A43:K43"/>
+    <mergeCell ref="A44:K44"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="A36:K36"/>
+    <mergeCell ref="A37:K37"/>
+    <mergeCell ref="A38:K38"/>
+    <mergeCell ref="A39:K39"/>
+    <mergeCell ref="A40:K40"/>
+    <mergeCell ref="B1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="G3:K3"/>
+    <mergeCell ref="A31:K31"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A32" r:id="rId1"/>
@@ -25500,25 +25500,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="424" t="s">
+      <c r="A1" s="419" t="s">
         <v>177</v>
       </c>
-      <c r="B1" s="424"/>
-      <c r="C1" s="424"/>
-      <c r="D1" s="424"/>
-      <c r="E1" s="424"/>
-      <c r="F1" s="424"/>
-      <c r="G1" s="424"/>
-      <c r="H1" s="424"/>
-      <c r="I1" s="424"/>
-      <c r="J1" s="424"/>
-      <c r="K1" s="424"/>
-      <c r="L1" s="424"/>
-      <c r="M1" s="424"/>
-      <c r="N1" s="424"/>
-      <c r="O1" s="424"/>
-      <c r="P1" s="424"/>
-      <c r="Q1" s="424"/>
+      <c r="B1" s="419"/>
+      <c r="C1" s="419"/>
+      <c r="D1" s="419"/>
+      <c r="E1" s="419"/>
+      <c r="F1" s="419"/>
+      <c r="G1" s="419"/>
+      <c r="H1" s="419"/>
+      <c r="I1" s="419"/>
+      <c r="J1" s="419"/>
+      <c r="K1" s="419"/>
+      <c r="L1" s="419"/>
+      <c r="M1" s="419"/>
+      <c r="N1" s="419"/>
+      <c r="O1" s="419"/>
+      <c r="P1" s="419"/>
+      <c r="Q1" s="419"/>
       <c r="R1" s="6"/>
       <c r="S1" s="6"/>
       <c r="T1" s="114"/>
@@ -25541,26 +25541,26 @@
     </row>
     <row r="2" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="116"/>
-      <c r="B2" s="425" t="s">
+      <c r="B2" s="420" t="s">
         <v>178</v>
       </c>
-      <c r="C2" s="425"/>
-      <c r="D2" s="425"/>
-      <c r="E2" s="425"/>
-      <c r="F2" s="425"/>
-      <c r="G2" s="425"/>
-      <c r="H2" s="425"/>
-      <c r="I2" s="425"/>
-      <c r="J2" s="425"/>
-      <c r="K2" s="425"/>
-      <c r="L2" s="425"/>
-      <c r="M2" s="425"/>
+      <c r="C2" s="420"/>
+      <c r="D2" s="420"/>
+      <c r="E2" s="420"/>
+      <c r="F2" s="420"/>
+      <c r="G2" s="420"/>
+      <c r="H2" s="420"/>
+      <c r="I2" s="420"/>
+      <c r="J2" s="420"/>
+      <c r="K2" s="420"/>
+      <c r="L2" s="420"/>
+      <c r="M2" s="420"/>
       <c r="N2" s="24"/>
       <c r="O2" s="24"/>
-      <c r="P2" s="426" t="s">
+      <c r="P2" s="421" t="s">
         <v>179</v>
       </c>
-      <c r="Q2" s="426"/>
+      <c r="Q2" s="421"/>
       <c r="R2" s="117"/>
       <c r="S2" s="6"/>
       <c r="T2" s="114"/>
@@ -25583,36 +25583,36 @@
     </row>
     <row r="3" spans="1:36" s="7" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="118"/>
-      <c r="B3" s="427" t="s">
+      <c r="B3" s="422" t="s">
         <v>180</v>
       </c>
-      <c r="C3" s="427"/>
-      <c r="D3" s="428" t="s">
+      <c r="C3" s="422"/>
+      <c r="D3" s="423" t="s">
         <v>181</v>
       </c>
-      <c r="E3" s="428"/>
-      <c r="F3" s="429" t="s">
+      <c r="E3" s="423"/>
+      <c r="F3" s="424" t="s">
         <v>182</v>
       </c>
-      <c r="G3" s="429"/>
-      <c r="H3" s="428" t="s">
+      <c r="G3" s="424"/>
+      <c r="H3" s="423" t="s">
         <v>183</v>
       </c>
-      <c r="I3" s="428"/>
-      <c r="J3" s="429" t="s">
+      <c r="I3" s="423"/>
+      <c r="J3" s="424" t="s">
         <v>184</v>
       </c>
-      <c r="K3" s="429"/>
-      <c r="L3" s="430" t="s">
+      <c r="K3" s="424"/>
+      <c r="L3" s="425" t="s">
         <v>185</v>
       </c>
-      <c r="M3" s="430"/>
-      <c r="N3" s="431" t="s">
+      <c r="M3" s="425"/>
+      <c r="N3" s="426" t="s">
         <v>186</v>
       </c>
-      <c r="O3" s="431"/>
-      <c r="P3" s="426"/>
-      <c r="Q3" s="426"/>
+      <c r="O3" s="426"/>
+      <c r="P3" s="421"/>
+      <c r="Q3" s="421"/>
       <c r="R3" s="117"/>
       <c r="S3" s="6"/>
       <c r="T3" s="114"/>
@@ -25686,27 +25686,27 @@
         <v>189</v>
       </c>
       <c r="R4" s="117"/>
-      <c r="S4" s="420" t="s">
+      <c r="S4" s="427" t="s">
         <v>190</v>
       </c>
-      <c r="T4" s="420"/>
-      <c r="U4" s="420"/>
-      <c r="V4" s="420"/>
-      <c r="W4" s="420"/>
-      <c r="X4" s="420"/>
-      <c r="Y4" s="420"/>
-      <c r="Z4" s="420"/>
+      <c r="T4" s="427"/>
+      <c r="U4" s="427"/>
+      <c r="V4" s="427"/>
+      <c r="W4" s="427"/>
+      <c r="X4" s="427"/>
+      <c r="Y4" s="427"/>
+      <c r="Z4" s="427"/>
       <c r="AA4" s="6"/>
-      <c r="AB4" s="420" t="s">
+      <c r="AB4" s="427" t="s">
         <v>191</v>
       </c>
-      <c r="AC4" s="420"/>
-      <c r="AD4" s="420"/>
-      <c r="AE4" s="420"/>
-      <c r="AF4" s="420"/>
-      <c r="AG4" s="420"/>
-      <c r="AH4" s="420"/>
-      <c r="AI4" s="420"/>
+      <c r="AC4" s="427"/>
+      <c r="AD4" s="427"/>
+      <c r="AE4" s="427"/>
+      <c r="AF4" s="427"/>
+      <c r="AG4" s="427"/>
+      <c r="AH4" s="427"/>
+      <c r="AI4" s="427"/>
       <c r="AJ4" s="6"/>
     </row>
     <row r="5" spans="1:36" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -30012,25 +30012,25 @@
       <c r="AJ48" s="6"/>
     </row>
     <row r="49" spans="1:36" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="421" t="s">
+      <c r="A49" s="428" t="s">
         <v>218</v>
       </c>
-      <c r="B49" s="421"/>
-      <c r="C49" s="421"/>
-      <c r="D49" s="421"/>
-      <c r="E49" s="421"/>
-      <c r="F49" s="421"/>
-      <c r="G49" s="421"/>
-      <c r="H49" s="421"/>
-      <c r="I49" s="421"/>
-      <c r="J49" s="421"/>
-      <c r="K49" s="421"/>
-      <c r="L49" s="421"/>
-      <c r="M49" s="421"/>
-      <c r="N49" s="421"/>
-      <c r="O49" s="421"/>
-      <c r="P49" s="421"/>
-      <c r="Q49" s="421"/>
+      <c r="B49" s="428"/>
+      <c r="C49" s="428"/>
+      <c r="D49" s="428"/>
+      <c r="E49" s="428"/>
+      <c r="F49" s="428"/>
+      <c r="G49" s="428"/>
+      <c r="H49" s="428"/>
+      <c r="I49" s="428"/>
+      <c r="J49" s="428"/>
+      <c r="K49" s="428"/>
+      <c r="L49" s="428"/>
+      <c r="M49" s="428"/>
+      <c r="N49" s="428"/>
+      <c r="O49" s="428"/>
+      <c r="P49" s="428"/>
+      <c r="Q49" s="428"/>
       <c r="R49" s="6"/>
       <c r="S49" s="6"/>
       <c r="T49" s="114"/>
@@ -30090,25 +30090,25 @@
       <c r="AJ50" s="6"/>
     </row>
     <row r="51" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="422" t="s">
+      <c r="A51" s="429" t="s">
         <v>219</v>
       </c>
-      <c r="B51" s="422"/>
-      <c r="C51" s="422"/>
-      <c r="D51" s="422"/>
-      <c r="E51" s="422"/>
-      <c r="F51" s="422"/>
-      <c r="G51" s="422"/>
-      <c r="H51" s="422"/>
-      <c r="I51" s="422"/>
-      <c r="J51" s="422"/>
-      <c r="K51" s="422"/>
-      <c r="L51" s="422"/>
-      <c r="M51" s="422"/>
-      <c r="N51" s="422"/>
-      <c r="O51" s="422"/>
-      <c r="P51" s="422"/>
-      <c r="Q51" s="422"/>
+      <c r="B51" s="429"/>
+      <c r="C51" s="429"/>
+      <c r="D51" s="429"/>
+      <c r="E51" s="429"/>
+      <c r="F51" s="429"/>
+      <c r="G51" s="429"/>
+      <c r="H51" s="429"/>
+      <c r="I51" s="429"/>
+      <c r="J51" s="429"/>
+      <c r="K51" s="429"/>
+      <c r="L51" s="429"/>
+      <c r="M51" s="429"/>
+      <c r="N51" s="429"/>
+      <c r="O51" s="429"/>
+      <c r="P51" s="429"/>
+      <c r="Q51" s="429"/>
       <c r="R51" s="6"/>
       <c r="S51" s="6"/>
       <c r="T51" s="114"/>
@@ -30130,25 +30130,25 @@
       <c r="AJ51" s="6"/>
     </row>
     <row r="52" spans="1:36" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="423" t="s">
+      <c r="A52" s="430" t="s">
         <v>220</v>
       </c>
-      <c r="B52" s="423"/>
-      <c r="C52" s="423"/>
-      <c r="D52" s="423"/>
-      <c r="E52" s="423"/>
-      <c r="F52" s="423"/>
-      <c r="G52" s="423"/>
-      <c r="H52" s="423"/>
-      <c r="I52" s="423"/>
-      <c r="J52" s="423"/>
-      <c r="K52" s="423"/>
-      <c r="L52" s="423"/>
-      <c r="M52" s="423"/>
-      <c r="N52" s="423"/>
-      <c r="O52" s="423"/>
-      <c r="P52" s="423"/>
-      <c r="Q52" s="423"/>
+      <c r="B52" s="430"/>
+      <c r="C52" s="430"/>
+      <c r="D52" s="430"/>
+      <c r="E52" s="430"/>
+      <c r="F52" s="430"/>
+      <c r="G52" s="430"/>
+      <c r="H52" s="430"/>
+      <c r="I52" s="430"/>
+      <c r="J52" s="430"/>
+      <c r="K52" s="430"/>
+      <c r="L52" s="430"/>
+      <c r="M52" s="430"/>
+      <c r="N52" s="430"/>
+      <c r="O52" s="430"/>
+      <c r="P52" s="430"/>
+      <c r="Q52" s="430"/>
       <c r="R52" s="6"/>
       <c r="S52" s="6"/>
       <c r="T52" s="114"/>
@@ -30169,25 +30169,25 @@
       <c r="AI52" s="115"/>
     </row>
     <row r="53" spans="1:36" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="419" t="s">
+      <c r="A53" s="431" t="s">
         <v>221</v>
       </c>
-      <c r="B53" s="419"/>
-      <c r="C53" s="419"/>
-      <c r="D53" s="419"/>
-      <c r="E53" s="419"/>
-      <c r="F53" s="419"/>
-      <c r="G53" s="419"/>
-      <c r="H53" s="419"/>
-      <c r="I53" s="419"/>
-      <c r="J53" s="419"/>
-      <c r="K53" s="419"/>
-      <c r="L53" s="419"/>
-      <c r="M53" s="419"/>
-      <c r="N53" s="419"/>
-      <c r="O53" s="419"/>
-      <c r="P53" s="419"/>
-      <c r="Q53" s="419"/>
+      <c r="B53" s="431"/>
+      <c r="C53" s="431"/>
+      <c r="D53" s="431"/>
+      <c r="E53" s="431"/>
+      <c r="F53" s="431"/>
+      <c r="G53" s="431"/>
+      <c r="H53" s="431"/>
+      <c r="I53" s="431"/>
+      <c r="J53" s="431"/>
+      <c r="K53" s="431"/>
+      <c r="L53" s="431"/>
+      <c r="M53" s="431"/>
+      <c r="N53" s="431"/>
+      <c r="O53" s="431"/>
+      <c r="P53" s="431"/>
+      <c r="Q53" s="431"/>
       <c r="R53" s="6"/>
       <c r="S53" s="6"/>
       <c r="T53" s="114"/>
@@ -30208,25 +30208,25 @@
       <c r="AI53" s="115"/>
     </row>
     <row r="54" spans="1:36" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="409" t="s">
+      <c r="A54" s="418" t="s">
         <v>222</v>
       </c>
-      <c r="B54" s="409"/>
-      <c r="C54" s="409"/>
-      <c r="D54" s="409"/>
-      <c r="E54" s="409"/>
-      <c r="F54" s="409"/>
-      <c r="G54" s="409"/>
-      <c r="H54" s="409"/>
-      <c r="I54" s="409"/>
-      <c r="J54" s="409"/>
-      <c r="K54" s="409"/>
-      <c r="L54" s="409"/>
-      <c r="M54" s="409"/>
-      <c r="N54" s="409"/>
-      <c r="O54" s="409"/>
-      <c r="P54" s="409"/>
-      <c r="Q54" s="409"/>
+      <c r="B54" s="418"/>
+      <c r="C54" s="418"/>
+      <c r="D54" s="418"/>
+      <c r="E54" s="418"/>
+      <c r="F54" s="418"/>
+      <c r="G54" s="418"/>
+      <c r="H54" s="418"/>
+      <c r="I54" s="418"/>
+      <c r="J54" s="418"/>
+      <c r="K54" s="418"/>
+      <c r="L54" s="418"/>
+      <c r="M54" s="418"/>
+      <c r="N54" s="418"/>
+      <c r="O54" s="418"/>
+      <c r="P54" s="418"/>
+      <c r="Q54" s="418"/>
       <c r="R54" s="6"/>
       <c r="S54" s="6"/>
       <c r="T54" s="114"/>
@@ -30247,25 +30247,25 @@
       <c r="AI54" s="115"/>
     </row>
     <row r="55" spans="1:36" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="409" t="s">
+      <c r="A55" s="418" t="s">
         <v>223</v>
       </c>
-      <c r="B55" s="409"/>
-      <c r="C55" s="409"/>
-      <c r="D55" s="409"/>
-      <c r="E55" s="409"/>
-      <c r="F55" s="409"/>
-      <c r="G55" s="409"/>
-      <c r="H55" s="409"/>
-      <c r="I55" s="409"/>
-      <c r="J55" s="409"/>
-      <c r="K55" s="409"/>
-      <c r="L55" s="409"/>
-      <c r="M55" s="409"/>
-      <c r="N55" s="409"/>
-      <c r="O55" s="409"/>
-      <c r="P55" s="409"/>
-      <c r="Q55" s="409"/>
+      <c r="B55" s="418"/>
+      <c r="C55" s="418"/>
+      <c r="D55" s="418"/>
+      <c r="E55" s="418"/>
+      <c r="F55" s="418"/>
+      <c r="G55" s="418"/>
+      <c r="H55" s="418"/>
+      <c r="I55" s="418"/>
+      <c r="J55" s="418"/>
+      <c r="K55" s="418"/>
+      <c r="L55" s="418"/>
+      <c r="M55" s="418"/>
+      <c r="N55" s="418"/>
+      <c r="O55" s="418"/>
+      <c r="P55" s="418"/>
+      <c r="Q55" s="418"/>
       <c r="R55" s="6"/>
       <c r="S55" s="6"/>
       <c r="T55" s="114"/>
@@ -30286,25 +30286,25 @@
       <c r="AI55" s="115"/>
     </row>
     <row r="56" spans="1:36" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="409" t="s">
+      <c r="A56" s="418" t="s">
         <v>224</v>
       </c>
-      <c r="B56" s="409"/>
-      <c r="C56" s="409"/>
-      <c r="D56" s="409"/>
-      <c r="E56" s="409"/>
-      <c r="F56" s="409"/>
-      <c r="G56" s="409"/>
-      <c r="H56" s="409"/>
-      <c r="I56" s="409"/>
-      <c r="J56" s="409"/>
-      <c r="K56" s="409"/>
-      <c r="L56" s="409"/>
-      <c r="M56" s="409"/>
-      <c r="N56" s="409"/>
-      <c r="O56" s="409"/>
-      <c r="P56" s="409"/>
-      <c r="Q56" s="409"/>
+      <c r="B56" s="418"/>
+      <c r="C56" s="418"/>
+      <c r="D56" s="418"/>
+      <c r="E56" s="418"/>
+      <c r="F56" s="418"/>
+      <c r="G56" s="418"/>
+      <c r="H56" s="418"/>
+      <c r="I56" s="418"/>
+      <c r="J56" s="418"/>
+      <c r="K56" s="418"/>
+      <c r="L56" s="418"/>
+      <c r="M56" s="418"/>
+      <c r="N56" s="418"/>
+      <c r="O56" s="418"/>
+      <c r="P56" s="418"/>
+      <c r="Q56" s="418"/>
       <c r="R56" s="6"/>
       <c r="S56" s="6"/>
       <c r="T56" s="114"/>
@@ -30325,25 +30325,25 @@
       <c r="AI56" s="115"/>
     </row>
     <row r="57" spans="1:36" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="409" t="s">
+      <c r="A57" s="418" t="s">
         <v>225</v>
       </c>
-      <c r="B57" s="409"/>
-      <c r="C57" s="409"/>
-      <c r="D57" s="409"/>
-      <c r="E57" s="409"/>
-      <c r="F57" s="409"/>
-      <c r="G57" s="409"/>
-      <c r="H57" s="409"/>
-      <c r="I57" s="409"/>
-      <c r="J57" s="409"/>
-      <c r="K57" s="409"/>
-      <c r="L57" s="409"/>
-      <c r="M57" s="409"/>
-      <c r="N57" s="409"/>
-      <c r="O57" s="409"/>
-      <c r="P57" s="409"/>
-      <c r="Q57" s="409"/>
+      <c r="B57" s="418"/>
+      <c r="C57" s="418"/>
+      <c r="D57" s="418"/>
+      <c r="E57" s="418"/>
+      <c r="F57" s="418"/>
+      <c r="G57" s="418"/>
+      <c r="H57" s="418"/>
+      <c r="I57" s="418"/>
+      <c r="J57" s="418"/>
+      <c r="K57" s="418"/>
+      <c r="L57" s="418"/>
+      <c r="M57" s="418"/>
+      <c r="N57" s="418"/>
+      <c r="O57" s="418"/>
+      <c r="P57" s="418"/>
+      <c r="Q57" s="418"/>
       <c r="R57" s="6"/>
       <c r="S57" s="6"/>
       <c r="T57" s="114"/>
@@ -30364,25 +30364,25 @@
       <c r="AI57" s="115"/>
     </row>
     <row r="58" spans="1:36" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="409" t="s">
+      <c r="A58" s="418" t="s">
         <v>226</v>
       </c>
-      <c r="B58" s="409"/>
-      <c r="C58" s="409"/>
-      <c r="D58" s="409"/>
-      <c r="E58" s="409"/>
-      <c r="F58" s="409"/>
-      <c r="G58" s="409"/>
-      <c r="H58" s="409"/>
-      <c r="I58" s="409"/>
-      <c r="J58" s="409"/>
-      <c r="K58" s="409"/>
-      <c r="L58" s="409"/>
-      <c r="M58" s="409"/>
-      <c r="N58" s="409"/>
-      <c r="O58" s="409"/>
-      <c r="P58" s="409"/>
-      <c r="Q58" s="409"/>
+      <c r="B58" s="418"/>
+      <c r="C58" s="418"/>
+      <c r="D58" s="418"/>
+      <c r="E58" s="418"/>
+      <c r="F58" s="418"/>
+      <c r="G58" s="418"/>
+      <c r="H58" s="418"/>
+      <c r="I58" s="418"/>
+      <c r="J58" s="418"/>
+      <c r="K58" s="418"/>
+      <c r="L58" s="418"/>
+      <c r="M58" s="418"/>
+      <c r="N58" s="418"/>
+      <c r="O58" s="418"/>
+      <c r="P58" s="418"/>
+      <c r="Q58" s="418"/>
       <c r="R58" s="6"/>
       <c r="S58" s="6"/>
       <c r="T58" s="114"/>
@@ -30403,25 +30403,25 @@
       <c r="AI58" s="115"/>
     </row>
     <row r="59" spans="1:36" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="409" t="s">
+      <c r="A59" s="418" t="s">
         <v>227</v>
       </c>
-      <c r="B59" s="409"/>
-      <c r="C59" s="409"/>
-      <c r="D59" s="409"/>
-      <c r="E59" s="409"/>
-      <c r="F59" s="409"/>
-      <c r="G59" s="409"/>
-      <c r="H59" s="409"/>
-      <c r="I59" s="409"/>
-      <c r="J59" s="409"/>
-      <c r="K59" s="409"/>
-      <c r="L59" s="409"/>
-      <c r="M59" s="409"/>
-      <c r="N59" s="409"/>
-      <c r="O59" s="409"/>
-      <c r="P59" s="409"/>
-      <c r="Q59" s="409"/>
+      <c r="B59" s="418"/>
+      <c r="C59" s="418"/>
+      <c r="D59" s="418"/>
+      <c r="E59" s="418"/>
+      <c r="F59" s="418"/>
+      <c r="G59" s="418"/>
+      <c r="H59" s="418"/>
+      <c r="I59" s="418"/>
+      <c r="J59" s="418"/>
+      <c r="K59" s="418"/>
+      <c r="L59" s="418"/>
+      <c r="M59" s="418"/>
+      <c r="N59" s="418"/>
+      <c r="O59" s="418"/>
+      <c r="P59" s="418"/>
+      <c r="Q59" s="418"/>
       <c r="R59" s="6"/>
       <c r="S59" s="6"/>
       <c r="T59" s="114"/>
@@ -30442,25 +30442,25 @@
       <c r="AI59" s="115"/>
     </row>
     <row r="60" spans="1:36" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="409" t="s">
+      <c r="A60" s="418" t="s">
         <v>228</v>
       </c>
-      <c r="B60" s="409"/>
-      <c r="C60" s="409"/>
-      <c r="D60" s="409"/>
-      <c r="E60" s="409"/>
-      <c r="F60" s="409"/>
-      <c r="G60" s="409"/>
-      <c r="H60" s="409"/>
-      <c r="I60" s="409"/>
-      <c r="J60" s="409"/>
-      <c r="K60" s="409"/>
-      <c r="L60" s="409"/>
-      <c r="M60" s="409"/>
-      <c r="N60" s="409"/>
-      <c r="O60" s="409"/>
-      <c r="P60" s="409"/>
-      <c r="Q60" s="409"/>
+      <c r="B60" s="418"/>
+      <c r="C60" s="418"/>
+      <c r="D60" s="418"/>
+      <c r="E60" s="418"/>
+      <c r="F60" s="418"/>
+      <c r="G60" s="418"/>
+      <c r="H60" s="418"/>
+      <c r="I60" s="418"/>
+      <c r="J60" s="418"/>
+      <c r="K60" s="418"/>
+      <c r="L60" s="418"/>
+      <c r="M60" s="418"/>
+      <c r="N60" s="418"/>
+      <c r="O60" s="418"/>
+      <c r="P60" s="418"/>
+      <c r="Q60" s="418"/>
       <c r="R60" s="6"/>
       <c r="S60" s="6"/>
       <c r="T60" s="114"/>
@@ -30481,25 +30481,25 @@
       <c r="AI60" s="115"/>
     </row>
     <row r="61" spans="1:36" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="409" t="s">
+      <c r="A61" s="418" t="s">
         <v>229</v>
       </c>
-      <c r="B61" s="409"/>
-      <c r="C61" s="409"/>
-      <c r="D61" s="409"/>
-      <c r="E61" s="409"/>
-      <c r="F61" s="409"/>
-      <c r="G61" s="409"/>
-      <c r="H61" s="409"/>
-      <c r="I61" s="409"/>
-      <c r="J61" s="409"/>
-      <c r="K61" s="409"/>
-      <c r="L61" s="409"/>
-      <c r="M61" s="409"/>
-      <c r="N61" s="409"/>
-      <c r="O61" s="409"/>
-      <c r="P61" s="409"/>
-      <c r="Q61" s="409"/>
+      <c r="B61" s="418"/>
+      <c r="C61" s="418"/>
+      <c r="D61" s="418"/>
+      <c r="E61" s="418"/>
+      <c r="F61" s="418"/>
+      <c r="G61" s="418"/>
+      <c r="H61" s="418"/>
+      <c r="I61" s="418"/>
+      <c r="J61" s="418"/>
+      <c r="K61" s="418"/>
+      <c r="L61" s="418"/>
+      <c r="M61" s="418"/>
+      <c r="N61" s="418"/>
+      <c r="O61" s="418"/>
+      <c r="P61" s="418"/>
+      <c r="Q61" s="418"/>
       <c r="R61" s="6"/>
       <c r="S61" s="6"/>
       <c r="T61" s="114"/>
@@ -30520,25 +30520,25 @@
       <c r="AI61" s="115"/>
     </row>
     <row r="62" spans="1:36" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="409" t="s">
+      <c r="A62" s="418" t="s">
         <v>230</v>
       </c>
-      <c r="B62" s="409"/>
-      <c r="C62" s="409"/>
-      <c r="D62" s="409"/>
-      <c r="E62" s="409"/>
-      <c r="F62" s="409"/>
-      <c r="G62" s="409"/>
-      <c r="H62" s="409"/>
-      <c r="I62" s="409"/>
-      <c r="J62" s="409"/>
-      <c r="K62" s="409"/>
-      <c r="L62" s="409"/>
-      <c r="M62" s="409"/>
-      <c r="N62" s="409"/>
-      <c r="O62" s="409"/>
-      <c r="P62" s="409"/>
-      <c r="Q62" s="409"/>
+      <c r="B62" s="418"/>
+      <c r="C62" s="418"/>
+      <c r="D62" s="418"/>
+      <c r="E62" s="418"/>
+      <c r="F62" s="418"/>
+      <c r="G62" s="418"/>
+      <c r="H62" s="418"/>
+      <c r="I62" s="418"/>
+      <c r="J62" s="418"/>
+      <c r="K62" s="418"/>
+      <c r="L62" s="418"/>
+      <c r="M62" s="418"/>
+      <c r="N62" s="418"/>
+      <c r="O62" s="418"/>
+      <c r="P62" s="418"/>
+      <c r="Q62" s="418"/>
       <c r="R62" s="6"/>
       <c r="S62" s="6"/>
       <c r="T62" s="114"/>
@@ -30559,25 +30559,25 @@
       <c r="AI62" s="115"/>
     </row>
     <row r="63" spans="1:36" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="409" t="s">
+      <c r="A63" s="418" t="s">
         <v>231</v>
       </c>
-      <c r="B63" s="409"/>
-      <c r="C63" s="409"/>
-      <c r="D63" s="409"/>
-      <c r="E63" s="409"/>
-      <c r="F63" s="409"/>
-      <c r="G63" s="409"/>
-      <c r="H63" s="409"/>
-      <c r="I63" s="409"/>
-      <c r="J63" s="409"/>
-      <c r="K63" s="409"/>
-      <c r="L63" s="409"/>
-      <c r="M63" s="409"/>
-      <c r="N63" s="409"/>
-      <c r="O63" s="409"/>
-      <c r="P63" s="409"/>
-      <c r="Q63" s="409"/>
+      <c r="B63" s="418"/>
+      <c r="C63" s="418"/>
+      <c r="D63" s="418"/>
+      <c r="E63" s="418"/>
+      <c r="F63" s="418"/>
+      <c r="G63" s="418"/>
+      <c r="H63" s="418"/>
+      <c r="I63" s="418"/>
+      <c r="J63" s="418"/>
+      <c r="K63" s="418"/>
+      <c r="L63" s="418"/>
+      <c r="M63" s="418"/>
+      <c r="N63" s="418"/>
+      <c r="O63" s="418"/>
+      <c r="P63" s="418"/>
+      <c r="Q63" s="418"/>
       <c r="R63" s="6"/>
       <c r="S63" s="6"/>
       <c r="T63" s="114"/>
@@ -30598,25 +30598,25 @@
       <c r="AI63" s="115"/>
     </row>
     <row r="64" spans="1:36" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="409" t="s">
+      <c r="A64" s="418" t="s">
         <v>232</v>
       </c>
-      <c r="B64" s="409"/>
-      <c r="C64" s="409"/>
-      <c r="D64" s="409"/>
-      <c r="E64" s="409"/>
-      <c r="F64" s="409"/>
-      <c r="G64" s="409"/>
-      <c r="H64" s="409"/>
-      <c r="I64" s="409"/>
-      <c r="J64" s="409"/>
-      <c r="K64" s="409"/>
-      <c r="L64" s="409"/>
-      <c r="M64" s="409"/>
-      <c r="N64" s="409"/>
-      <c r="O64" s="409"/>
-      <c r="P64" s="409"/>
-      <c r="Q64" s="409"/>
+      <c r="B64" s="418"/>
+      <c r="C64" s="418"/>
+      <c r="D64" s="418"/>
+      <c r="E64" s="418"/>
+      <c r="F64" s="418"/>
+      <c r="G64" s="418"/>
+      <c r="H64" s="418"/>
+      <c r="I64" s="418"/>
+      <c r="J64" s="418"/>
+      <c r="K64" s="418"/>
+      <c r="L64" s="418"/>
+      <c r="M64" s="418"/>
+      <c r="N64" s="418"/>
+      <c r="O64" s="418"/>
+      <c r="P64" s="418"/>
+      <c r="Q64" s="418"/>
       <c r="R64" s="6"/>
       <c r="S64" s="6"/>
       <c r="T64" s="114"/>
@@ -30637,25 +30637,25 @@
       <c r="AI64" s="115"/>
     </row>
     <row r="65" spans="1:35" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="409" t="s">
+      <c r="A65" s="418" t="s">
         <v>233</v>
       </c>
-      <c r="B65" s="409"/>
-      <c r="C65" s="409"/>
-      <c r="D65" s="409"/>
-      <c r="E65" s="409"/>
-      <c r="F65" s="409"/>
-      <c r="G65" s="409"/>
-      <c r="H65" s="409"/>
-      <c r="I65" s="409"/>
-      <c r="J65" s="409"/>
-      <c r="K65" s="409"/>
-      <c r="L65" s="409"/>
-      <c r="M65" s="409"/>
-      <c r="N65" s="409"/>
-      <c r="O65" s="409"/>
-      <c r="P65" s="409"/>
-      <c r="Q65" s="409"/>
+      <c r="B65" s="418"/>
+      <c r="C65" s="418"/>
+      <c r="D65" s="418"/>
+      <c r="E65" s="418"/>
+      <c r="F65" s="418"/>
+      <c r="G65" s="418"/>
+      <c r="H65" s="418"/>
+      <c r="I65" s="418"/>
+      <c r="J65" s="418"/>
+      <c r="K65" s="418"/>
+      <c r="L65" s="418"/>
+      <c r="M65" s="418"/>
+      <c r="N65" s="418"/>
+      <c r="O65" s="418"/>
+      <c r="P65" s="418"/>
+      <c r="Q65" s="418"/>
       <c r="R65" s="6"/>
       <c r="S65" s="6"/>
       <c r="T65" s="114"/>
@@ -30676,25 +30676,25 @@
       <c r="AI65" s="115"/>
     </row>
     <row r="66" spans="1:35" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="409" t="s">
+      <c r="A66" s="418" t="s">
         <v>234</v>
       </c>
-      <c r="B66" s="409"/>
-      <c r="C66" s="409"/>
-      <c r="D66" s="409"/>
-      <c r="E66" s="409"/>
-      <c r="F66" s="409"/>
-      <c r="G66" s="409"/>
-      <c r="H66" s="409"/>
-      <c r="I66" s="409"/>
-      <c r="J66" s="409"/>
-      <c r="K66" s="409"/>
-      <c r="L66" s="409"/>
-      <c r="M66" s="409"/>
-      <c r="N66" s="409"/>
-      <c r="O66" s="409"/>
-      <c r="P66" s="409"/>
-      <c r="Q66" s="409"/>
+      <c r="B66" s="418"/>
+      <c r="C66" s="418"/>
+      <c r="D66" s="418"/>
+      <c r="E66" s="418"/>
+      <c r="F66" s="418"/>
+      <c r="G66" s="418"/>
+      <c r="H66" s="418"/>
+      <c r="I66" s="418"/>
+      <c r="J66" s="418"/>
+      <c r="K66" s="418"/>
+      <c r="L66" s="418"/>
+      <c r="M66" s="418"/>
+      <c r="N66" s="418"/>
+      <c r="O66" s="418"/>
+      <c r="P66" s="418"/>
+      <c r="Q66" s="418"/>
       <c r="R66" s="6"/>
       <c r="S66" s="6"/>
       <c r="T66" s="114"/>
@@ -30715,23 +30715,23 @@
       <c r="AI66" s="115"/>
     </row>
     <row r="67" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="409"/>
-      <c r="B67" s="409"/>
-      <c r="C67" s="409"/>
-      <c r="D67" s="409"/>
-      <c r="E67" s="409"/>
-      <c r="F67" s="409"/>
-      <c r="G67" s="409"/>
-      <c r="H67" s="409"/>
-      <c r="I67" s="409"/>
-      <c r="J67" s="409"/>
-      <c r="K67" s="409"/>
-      <c r="L67" s="409"/>
-      <c r="M67" s="409"/>
-      <c r="N67" s="409"/>
-      <c r="O67" s="409"/>
-      <c r="P67" s="409"/>
-      <c r="Q67" s="409"/>
+      <c r="A67" s="418"/>
+      <c r="B67" s="418"/>
+      <c r="C67" s="418"/>
+      <c r="D67" s="418"/>
+      <c r="E67" s="418"/>
+      <c r="F67" s="418"/>
+      <c r="G67" s="418"/>
+      <c r="H67" s="418"/>
+      <c r="I67" s="418"/>
+      <c r="J67" s="418"/>
+      <c r="K67" s="418"/>
+      <c r="L67" s="418"/>
+      <c r="M67" s="418"/>
+      <c r="N67" s="418"/>
+      <c r="O67" s="418"/>
+      <c r="P67" s="418"/>
+      <c r="Q67" s="418"/>
       <c r="R67" s="6"/>
       <c r="S67" s="6"/>
       <c r="T67" s="114"/>
@@ -30752,25 +30752,25 @@
       <c r="AI67" s="115"/>
     </row>
     <row r="68" spans="1:35" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="406" t="s">
+      <c r="A68" s="417" t="s">
         <v>235</v>
       </c>
-      <c r="B68" s="406"/>
-      <c r="C68" s="406"/>
-      <c r="D68" s="406"/>
-      <c r="E68" s="406"/>
-      <c r="F68" s="406"/>
-      <c r="G68" s="406"/>
-      <c r="H68" s="406"/>
-      <c r="I68" s="406"/>
-      <c r="J68" s="406"/>
-      <c r="K68" s="406"/>
-      <c r="L68" s="406"/>
-      <c r="M68" s="406"/>
-      <c r="N68" s="406"/>
-      <c r="O68" s="406"/>
-      <c r="P68" s="406"/>
-      <c r="Q68" s="406"/>
+      <c r="B68" s="417"/>
+      <c r="C68" s="417"/>
+      <c r="D68" s="417"/>
+      <c r="E68" s="417"/>
+      <c r="F68" s="417"/>
+      <c r="G68" s="417"/>
+      <c r="H68" s="417"/>
+      <c r="I68" s="417"/>
+      <c r="J68" s="417"/>
+      <c r="K68" s="417"/>
+      <c r="L68" s="417"/>
+      <c r="M68" s="417"/>
+      <c r="N68" s="417"/>
+      <c r="O68" s="417"/>
+      <c r="P68" s="417"/>
+      <c r="Q68" s="417"/>
       <c r="R68" s="6"/>
       <c r="S68" s="6"/>
       <c r="T68" s="114"/>
@@ -30793,6 +30793,27 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="31">
+    <mergeCell ref="A68:Q68"/>
+    <mergeCell ref="A63:Q63"/>
+    <mergeCell ref="A64:Q64"/>
+    <mergeCell ref="A65:Q65"/>
+    <mergeCell ref="A66:Q66"/>
+    <mergeCell ref="A67:Q67"/>
+    <mergeCell ref="A58:Q58"/>
+    <mergeCell ref="A59:Q59"/>
+    <mergeCell ref="A60:Q60"/>
+    <mergeCell ref="A61:Q61"/>
+    <mergeCell ref="A62:Q62"/>
+    <mergeCell ref="A53:Q53"/>
+    <mergeCell ref="A54:Q54"/>
+    <mergeCell ref="A55:Q55"/>
+    <mergeCell ref="A56:Q56"/>
+    <mergeCell ref="A57:Q57"/>
+    <mergeCell ref="S4:Z4"/>
+    <mergeCell ref="AB4:AI4"/>
+    <mergeCell ref="A49:Q49"/>
+    <mergeCell ref="A51:Q51"/>
+    <mergeCell ref="A52:Q52"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="B2:M2"/>
     <mergeCell ref="P2:Q3"/>
@@ -30803,27 +30824,6 @@
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="N3:O3"/>
-    <mergeCell ref="S4:Z4"/>
-    <mergeCell ref="AB4:AI4"/>
-    <mergeCell ref="A49:Q49"/>
-    <mergeCell ref="A51:Q51"/>
-    <mergeCell ref="A52:Q52"/>
-    <mergeCell ref="A53:Q53"/>
-    <mergeCell ref="A54:Q54"/>
-    <mergeCell ref="A55:Q55"/>
-    <mergeCell ref="A56:Q56"/>
-    <mergeCell ref="A57:Q57"/>
-    <mergeCell ref="A58:Q58"/>
-    <mergeCell ref="A59:Q59"/>
-    <mergeCell ref="A60:Q60"/>
-    <mergeCell ref="A61:Q61"/>
-    <mergeCell ref="A62:Q62"/>
-    <mergeCell ref="A68:Q68"/>
-    <mergeCell ref="A63:Q63"/>
-    <mergeCell ref="A64:Q64"/>
-    <mergeCell ref="A65:Q65"/>
-    <mergeCell ref="A66:Q66"/>
-    <mergeCell ref="A67:Q67"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A68" r:id="rId1"/>
@@ -31797,13 +31797,13 @@
       <c r="R33" s="7"/>
     </row>
     <row r="34" spans="1:18" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="421" t="s">
+      <c r="A34" s="428" t="s">
         <v>247</v>
       </c>
-      <c r="B34" s="421"/>
-      <c r="C34" s="421"/>
-      <c r="D34" s="421"/>
-      <c r="E34" s="421"/>
+      <c r="B34" s="428"/>
+      <c r="C34" s="428"/>
+      <c r="D34" s="428"/>
+      <c r="E34" s="428"/>
       <c r="F34" s="6"/>
       <c r="G34" s="6"/>
       <c r="H34" s="6"/>
@@ -31852,13 +31852,13 @@
       <c r="R36" s="7"/>
     </row>
     <row r="37" spans="1:18" ht="139.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="419" t="s">
+      <c r="A37" s="431" t="s">
         <v>249</v>
       </c>
-      <c r="B37" s="419"/>
-      <c r="C37" s="419"/>
-      <c r="D37" s="419"/>
-      <c r="E37" s="419"/>
+      <c r="B37" s="431"/>
+      <c r="C37" s="431"/>
+      <c r="D37" s="431"/>
+      <c r="E37" s="431"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
       <c r="H37" s="6"/>
@@ -31874,13 +31874,13 @@
       <c r="R37" s="7"/>
     </row>
     <row r="38" spans="1:18" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="406" t="s">
+      <c r="A38" s="417" t="s">
         <v>250</v>
       </c>
-      <c r="B38" s="406"/>
-      <c r="C38" s="406"/>
-      <c r="D38" s="406"/>
-      <c r="E38" s="406"/>
+      <c r="B38" s="417"/>
+      <c r="C38" s="417"/>
+      <c r="D38" s="417"/>
+      <c r="E38" s="417"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
       <c r="H38" s="6"/>
@@ -32392,16 +32392,16 @@
       <c r="R16" s="7"/>
     </row>
     <row r="17" spans="1:18" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="421" t="s">
+      <c r="A17" s="428" t="s">
         <v>264</v>
       </c>
-      <c r="B17" s="421"/>
-      <c r="C17" s="421"/>
-      <c r="D17" s="421"/>
-      <c r="E17" s="421"/>
-      <c r="F17" s="421"/>
-      <c r="G17" s="421"/>
-      <c r="H17" s="421"/>
+      <c r="B17" s="428"/>
+      <c r="C17" s="428"/>
+      <c r="D17" s="428"/>
+      <c r="E17" s="428"/>
+      <c r="F17" s="428"/>
+      <c r="G17" s="428"/>
+      <c r="H17" s="428"/>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
@@ -32434,16 +32434,16 @@
       <c r="R18" s="7"/>
     </row>
     <row r="19" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="422" t="s">
+      <c r="A19" s="429" t="s">
         <v>265</v>
       </c>
-      <c r="B19" s="422"/>
-      <c r="C19" s="422"/>
-      <c r="D19" s="422"/>
-      <c r="E19" s="422"/>
-      <c r="F19" s="422"/>
-      <c r="G19" s="422"/>
-      <c r="H19" s="422"/>
+      <c r="B19" s="429"/>
+      <c r="C19" s="429"/>
+      <c r="D19" s="429"/>
+      <c r="E19" s="429"/>
+      <c r="F19" s="429"/>
+      <c r="G19" s="429"/>
+      <c r="H19" s="429"/>
       <c r="I19" s="76"/>
       <c r="J19" s="7"/>
       <c r="K19" s="7"/>
@@ -32456,16 +32456,16 @@
       <c r="R19" s="7"/>
     </row>
     <row r="20" spans="1:18" ht="93" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="419" t="s">
+      <c r="A20" s="431" t="s">
         <v>266</v>
       </c>
-      <c r="B20" s="419"/>
-      <c r="C20" s="419"/>
-      <c r="D20" s="419"/>
-      <c r="E20" s="419"/>
-      <c r="F20" s="419"/>
-      <c r="G20" s="419"/>
-      <c r="H20" s="419"/>
+      <c r="B20" s="431"/>
+      <c r="C20" s="431"/>
+      <c r="D20" s="431"/>
+      <c r="E20" s="431"/>
+      <c r="F20" s="431"/>
+      <c r="G20" s="431"/>
+      <c r="H20" s="431"/>
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
       <c r="K20" s="7"/>
@@ -32478,16 +32478,16 @@
       <c r="R20" s="7"/>
     </row>
     <row r="21" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="419" t="s">
+      <c r="A21" s="431" t="s">
         <v>267</v>
       </c>
-      <c r="B21" s="419"/>
-      <c r="C21" s="419"/>
-      <c r="D21" s="419"/>
-      <c r="E21" s="419"/>
-      <c r="F21" s="419"/>
-      <c r="G21" s="419"/>
-      <c r="H21" s="419"/>
+      <c r="B21" s="431"/>
+      <c r="C21" s="431"/>
+      <c r="D21" s="431"/>
+      <c r="E21" s="431"/>
+      <c r="F21" s="431"/>
+      <c r="G21" s="431"/>
+      <c r="H21" s="431"/>
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
       <c r="K21" s="7"/>
@@ -32500,16 +32500,16 @@
       <c r="R21" s="7"/>
     </row>
     <row r="22" spans="1:18" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="419" t="s">
+      <c r="A22" s="431" t="s">
         <v>268</v>
       </c>
-      <c r="B22" s="419"/>
-      <c r="C22" s="419"/>
-      <c r="D22" s="419"/>
-      <c r="E22" s="419"/>
-      <c r="F22" s="419"/>
-      <c r="G22" s="419"/>
-      <c r="H22" s="419"/>
+      <c r="B22" s="431"/>
+      <c r="C22" s="431"/>
+      <c r="D22" s="431"/>
+      <c r="E22" s="431"/>
+      <c r="F22" s="431"/>
+      <c r="G22" s="431"/>
+      <c r="H22" s="431"/>
       <c r="I22" s="76"/>
       <c r="J22" s="7"/>
       <c r="K22" s="7"/>
@@ -32522,16 +32522,16 @@
       <c r="R22" s="7"/>
     </row>
     <row r="23" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="419" t="s">
+      <c r="A23" s="431" t="s">
         <v>269</v>
       </c>
-      <c r="B23" s="419"/>
-      <c r="C23" s="419"/>
-      <c r="D23" s="419"/>
-      <c r="E23" s="419"/>
-      <c r="F23" s="419"/>
-      <c r="G23" s="419"/>
-      <c r="H23" s="419"/>
+      <c r="B23" s="431"/>
+      <c r="C23" s="431"/>
+      <c r="D23" s="431"/>
+      <c r="E23" s="431"/>
+      <c r="F23" s="431"/>
+      <c r="G23" s="431"/>
+      <c r="H23" s="431"/>
       <c r="I23" s="7"/>
       <c r="J23" s="7"/>
       <c r="K23" s="7"/>
@@ -32544,16 +32544,16 @@
       <c r="R23" s="7"/>
     </row>
     <row r="24" spans="1:18" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="410" t="s">
+      <c r="A24" s="413" t="s">
         <v>270</v>
       </c>
-      <c r="B24" s="410"/>
-      <c r="C24" s="410"/>
-      <c r="D24" s="410"/>
-      <c r="E24" s="410"/>
-      <c r="F24" s="410"/>
-      <c r="G24" s="410"/>
-      <c r="H24" s="410"/>
+      <c r="B24" s="413"/>
+      <c r="C24" s="413"/>
+      <c r="D24" s="413"/>
+      <c r="E24" s="413"/>
+      <c r="F24" s="413"/>
+      <c r="G24" s="413"/>
+      <c r="H24" s="413"/>
       <c r="I24" s="76"/>
       <c r="J24" s="7"/>
       <c r="K24" s="7"/>
@@ -32566,16 +32566,16 @@
       <c r="R24" s="7"/>
     </row>
     <row r="25" spans="1:18" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="419" t="s">
+      <c r="A25" s="431" t="s">
         <v>271</v>
       </c>
-      <c r="B25" s="419"/>
-      <c r="C25" s="419"/>
-      <c r="D25" s="419"/>
-      <c r="E25" s="419"/>
-      <c r="F25" s="419"/>
-      <c r="G25" s="419"/>
-      <c r="H25" s="419"/>
+      <c r="B25" s="431"/>
+      <c r="C25" s="431"/>
+      <c r="D25" s="431"/>
+      <c r="E25" s="431"/>
+      <c r="F25" s="431"/>
+      <c r="G25" s="431"/>
+      <c r="H25" s="431"/>
       <c r="I25" s="7"/>
       <c r="J25" s="7"/>
       <c r="K25" s="7"/>
@@ -32588,16 +32588,16 @@
       <c r="R25" s="7"/>
     </row>
     <row r="26" spans="1:18" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="419" t="s">
+      <c r="A26" s="431" t="s">
         <v>272</v>
       </c>
-      <c r="B26" s="419"/>
-      <c r="C26" s="419"/>
-      <c r="D26" s="419"/>
-      <c r="E26" s="419"/>
-      <c r="F26" s="419"/>
-      <c r="G26" s="419"/>
-      <c r="H26" s="419"/>
+      <c r="B26" s="431"/>
+      <c r="C26" s="431"/>
+      <c r="D26" s="431"/>
+      <c r="E26" s="431"/>
+      <c r="F26" s="431"/>
+      <c r="G26" s="431"/>
+      <c r="H26" s="431"/>
       <c r="I26" s="76"/>
       <c r="J26" s="7"/>
       <c r="K26" s="7"/>
@@ -32610,16 +32610,16 @@
       <c r="R26" s="7"/>
     </row>
     <row r="27" spans="1:18" ht="63" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="419" t="s">
+      <c r="A27" s="431" t="s">
         <v>273</v>
       </c>
-      <c r="B27" s="419"/>
-      <c r="C27" s="419"/>
-      <c r="D27" s="419"/>
-      <c r="E27" s="419"/>
-      <c r="F27" s="419"/>
-      <c r="G27" s="419"/>
-      <c r="H27" s="419"/>
+      <c r="B27" s="431"/>
+      <c r="C27" s="431"/>
+      <c r="D27" s="431"/>
+      <c r="E27" s="431"/>
+      <c r="F27" s="431"/>
+      <c r="G27" s="431"/>
+      <c r="H27" s="431"/>
       <c r="I27" s="7"/>
       <c r="J27" s="7"/>
       <c r="K27" s="7"/>
@@ -32632,16 +32632,16 @@
       <c r="R27" s="7"/>
     </row>
     <row r="28" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="419" t="s">
+      <c r="A28" s="431" t="s">
         <v>274</v>
       </c>
-      <c r="B28" s="419"/>
-      <c r="C28" s="419"/>
-      <c r="D28" s="419"/>
-      <c r="E28" s="419"/>
-      <c r="F28" s="419"/>
-      <c r="G28" s="419"/>
-      <c r="H28" s="419"/>
+      <c r="B28" s="431"/>
+      <c r="C28" s="431"/>
+      <c r="D28" s="431"/>
+      <c r="E28" s="431"/>
+      <c r="F28" s="431"/>
+      <c r="G28" s="431"/>
+      <c r="H28" s="431"/>
       <c r="I28" s="76"/>
       <c r="J28" s="7"/>
       <c r="K28" s="7"/>
@@ -32654,16 +32654,16 @@
       <c r="R28" s="7"/>
     </row>
     <row r="29" spans="1:18" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="406" t="s">
+      <c r="A29" s="417" t="s">
         <v>275</v>
       </c>
-      <c r="B29" s="406"/>
-      <c r="C29" s="406"/>
-      <c r="D29" s="406"/>
-      <c r="E29" s="406"/>
-      <c r="F29" s="406"/>
-      <c r="G29" s="406"/>
-      <c r="H29" s="406"/>
+      <c r="B29" s="417"/>
+      <c r="C29" s="417"/>
+      <c r="D29" s="417"/>
+      <c r="E29" s="417"/>
+      <c r="F29" s="417"/>
+      <c r="G29" s="417"/>
+      <c r="H29" s="417"/>
       <c r="I29" s="7"/>
       <c r="J29" s="7"/>
       <c r="K29" s="7"/>
@@ -32758,21 +32758,21 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="15">
+    <mergeCell ref="A25:H25"/>
+    <mergeCell ref="A26:H26"/>
+    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="A28:H28"/>
+    <mergeCell ref="A29:H29"/>
+    <mergeCell ref="A20:H20"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="A22:H22"/>
+    <mergeCell ref="A23:H23"/>
+    <mergeCell ref="A24:H24"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="A4:F4"/>
     <mergeCell ref="A17:H17"/>
     <mergeCell ref="A19:H19"/>
-    <mergeCell ref="A20:H20"/>
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="A22:H22"/>
-    <mergeCell ref="A23:H23"/>
-    <mergeCell ref="A24:H24"/>
-    <mergeCell ref="A25:H25"/>
-    <mergeCell ref="A26:H26"/>
-    <mergeCell ref="A27:H27"/>
-    <mergeCell ref="A28:H28"/>
-    <mergeCell ref="A29:H29"/>
   </mergeCells>
   <dataValidations count="8">
     <dataValidation type="whole" error="Please check this salary information as it is outside the normal range._x000a_" sqref="B7">
@@ -32828,7 +32828,7 @@
   <dimension ref="A1:AMK51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="A15" sqref="A15:G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -33091,14 +33091,16 @@
       <c r="B8" s="132"/>
       <c r="C8" s="133"/>
       <c r="D8" s="140"/>
-      <c r="E8" s="133"/>
+      <c r="E8" s="133">
+        <v>5</v>
+      </c>
       <c r="F8" s="140">
         <f t="shared" ref="F8:G10" si="0">SUM(B8,D8)</f>
         <v>0</v>
       </c>
       <c r="G8" s="133">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -33122,14 +33124,16 @@
       <c r="B9" s="148"/>
       <c r="C9" s="149"/>
       <c r="D9" s="152"/>
-      <c r="E9" s="149"/>
+      <c r="E9" s="149">
+        <v>5</v>
+      </c>
       <c r="F9" s="140">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G9" s="133">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -33153,14 +33157,16 @@
       <c r="B10" s="388"/>
       <c r="C10" s="389"/>
       <c r="D10" s="390"/>
-      <c r="E10" s="389"/>
+      <c r="E10" s="389">
+        <v>5</v>
+      </c>
       <c r="F10" s="140">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G10" s="391">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H10" s="62"/>
       <c r="I10" s="62"/>
@@ -33195,7 +33201,7 @@
       </c>
       <c r="E11" s="274">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F11" s="274">
         <f t="shared" si="1"/>
@@ -33203,7 +33209,7 @@
       </c>
       <c r="G11" s="274">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -33241,16 +33247,16 @@
       <c r="R12" s="6"/>
     </row>
     <row r="13" spans="1:21" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="421" t="s">
+      <c r="A13" s="428" t="s">
         <v>284</v>
       </c>
-      <c r="B13" s="421"/>
-      <c r="C13" s="421"/>
-      <c r="D13" s="421"/>
-      <c r="E13" s="421"/>
-      <c r="F13" s="421"/>
-      <c r="G13" s="421"/>
-      <c r="H13" s="421"/>
+      <c r="B13" s="428"/>
+      <c r="C13" s="428"/>
+      <c r="D13" s="428"/>
+      <c r="E13" s="428"/>
+      <c r="F13" s="428"/>
+      <c r="G13" s="428"/>
+      <c r="H13" s="428"/>
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
@@ -33283,15 +33289,15 @@
       <c r="R14" s="14"/>
     </row>
     <row r="15" spans="1:21" ht="107.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="423" t="s">
+      <c r="A15" s="430" t="s">
         <v>285</v>
       </c>
-      <c r="B15" s="423"/>
-      <c r="C15" s="423"/>
-      <c r="D15" s="423"/>
-      <c r="E15" s="423"/>
-      <c r="F15" s="423"/>
-      <c r="G15" s="423"/>
+      <c r="B15" s="430"/>
+      <c r="C15" s="430"/>
+      <c r="D15" s="430"/>
+      <c r="E15" s="430"/>
+      <c r="F15" s="430"/>
+      <c r="G15" s="430"/>
       <c r="H15" s="16"/>
       <c r="I15" s="16"/>
       <c r="J15" s="16"/>

</xml_diff>

<commit_message>
fix formulae in AAUP excel file
</commit_message>
<xml_diff>
--- a/data/imports/aaup-export.xlsx
+++ b/data/imports/aaup-export.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23540" windowHeight="14740" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23540" windowHeight="14740" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -6983,7 +6983,7 @@
   </sheetPr>
   <dimension ref="A1:AMK8036"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
@@ -25355,8 +25355,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="R38" sqref="R38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -30842,8 +30842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -31551,7 +31551,7 @@
         <v>0</v>
       </c>
       <c r="D26" s="255">
-        <f>D6+(D16*'Form 1'!$C$31)</f>
+        <f>D6+(D16*'Form 1'!$K$31)</f>
         <v>0</v>
       </c>
       <c r="E26" s="243">
@@ -31585,7 +31585,7 @@
         <v>0</v>
       </c>
       <c r="D27" s="257">
-        <f>D7+(D17*'Form 1'!$C$31)</f>
+        <f>D7+(D17*'Form 1'!$K$31)</f>
         <v>0</v>
       </c>
       <c r="E27" s="245">
@@ -31619,7 +31619,7 @@
         <v>0</v>
       </c>
       <c r="D28" s="255">
-        <f>D8+(D18*'Form 1'!$C$31)</f>
+        <f>D8+(D18*'Form 1'!$K$31)</f>
         <v>0</v>
       </c>
       <c r="E28" s="245">
@@ -31653,7 +31653,7 @@
         <v>0</v>
       </c>
       <c r="D29" s="257">
-        <f>D9+(D19*'Form 1'!$C$31)</f>
+        <f>D9+(D19*'Form 1'!$K$31)</f>
         <v>0</v>
       </c>
       <c r="E29" s="245">
@@ -31687,7 +31687,7 @@
         <v>0</v>
       </c>
       <c r="D30" s="255">
-        <f>D10+(D20*'Form 1'!$C$31)</f>
+        <f>D10+(D20*'Form 1'!$K$31)</f>
         <v>0</v>
       </c>
       <c r="E30" s="245">
@@ -31721,7 +31721,7 @@
         <v>0</v>
       </c>
       <c r="D31" s="257">
-        <f>D11+(D21*'Form 1'!$C$31)</f>
+        <f>D11+(D21*'Form 1'!$K$31)</f>
         <v>0</v>
       </c>
       <c r="E31" s="245">
@@ -31976,7 +31976,7 @@
       <c r="R42" s="7"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection password="EDAD" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="9">
     <mergeCell ref="A34:E34"/>
     <mergeCell ref="A36:E36"/>

</xml_diff>

<commit_message>
aaup excel template open tab 1 first
</commit_message>
<xml_diff>
--- a/data/imports/aaup-export.xlsx
+++ b/data/imports/aaup-export.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dfergu15/Documents/aaup/2017 prep/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/aaup/data/imports/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23540" windowHeight="14740" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23540" windowHeight="14740"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -4387,15 +4387,14 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="65" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="27" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="55" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="53" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -4413,14 +4412,42 @@
     <xf numFmtId="0" fontId="27" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="53" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="56" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4434,32 +4461,20 @@
     <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="56" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="31" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="57" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4484,21 +4499,6 @@
     </xf>
     <xf numFmtId="49" fontId="8" fillId="3" borderId="75" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -5140,7 +5140,7 @@
   </sheetPr>
   <dimension ref="A1:S50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -6983,7 +6983,7 @@
   </sheetPr>
   <dimension ref="A1:AMK8036"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
@@ -7007,18 +7007,18 @@
   <sheetData>
     <row r="1" spans="1:23" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="23"/>
-      <c r="B1" s="395" t="s">
+      <c r="B1" s="403" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="395"/>
-      <c r="D1" s="395"/>
-      <c r="E1" s="395"/>
-      <c r="F1" s="395"/>
-      <c r="G1" s="395"/>
-      <c r="H1" s="395"/>
-      <c r="I1" s="395"/>
-      <c r="J1" s="395"/>
-      <c r="K1" s="395"/>
+      <c r="C1" s="403"/>
+      <c r="D1" s="403"/>
+      <c r="E1" s="403"/>
+      <c r="F1" s="403"/>
+      <c r="G1" s="403"/>
+      <c r="H1" s="403"/>
+      <c r="I1" s="403"/>
+      <c r="J1" s="403"/>
+      <c r="K1" s="403"/>
       <c r="L1" s="6" t="s">
         <v>1</v>
       </c>
@@ -7036,15 +7036,15 @@
       </c>
     </row>
     <row r="2" spans="1:23" ht="23.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="396" t="s">
+      <c r="A2" s="404" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="396"/>
-      <c r="C2" s="396"/>
-      <c r="D2" s="396"/>
-      <c r="E2" s="396"/>
-      <c r="F2" s="396"/>
-      <c r="G2" s="396"/>
+      <c r="B2" s="404"/>
+      <c r="C2" s="404"/>
+      <c r="D2" s="404"/>
+      <c r="E2" s="404"/>
+      <c r="F2" s="404"/>
+      <c r="G2" s="404"/>
       <c r="H2" s="24"/>
       <c r="I2" s="24"/>
       <c r="J2" s="24"/>
@@ -7100,13 +7100,13 @@
       <c r="B5" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="397" t="s">
+      <c r="C5" s="405" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="397"/>
-      <c r="E5" s="397"/>
-      <c r="F5" s="397"/>
-      <c r="G5" s="397"/>
+      <c r="D5" s="405"/>
+      <c r="E5" s="405"/>
+      <c r="F5" s="405"/>
+      <c r="G5" s="405"/>
       <c r="H5" s="28"/>
       <c r="I5" s="28"/>
       <c r="J5" s="28"/>
@@ -8341,18 +8341,18 @@
       <c r="P61" s="6"/>
     </row>
     <row r="62" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="403" t="s">
+      <c r="A62" s="395" t="s">
         <v>86</v>
       </c>
-      <c r="B62" s="403"/>
-      <c r="C62" s="403"/>
-      <c r="D62" s="403"/>
-      <c r="E62" s="403"/>
-      <c r="F62" s="403"/>
-      <c r="G62" s="403"/>
-      <c r="H62" s="403"/>
-      <c r="I62" s="403"/>
-      <c r="J62" s="403"/>
+      <c r="B62" s="395"/>
+      <c r="C62" s="395"/>
+      <c r="D62" s="395"/>
+      <c r="E62" s="395"/>
+      <c r="F62" s="395"/>
+      <c r="G62" s="395"/>
+      <c r="H62" s="395"/>
+      <c r="I62" s="395"/>
+      <c r="J62" s="395"/>
       <c r="K62" s="6"/>
       <c r="L62" s="6"/>
       <c r="M62" s="6"/>
@@ -8361,18 +8361,18 @@
       <c r="P62" s="6"/>
     </row>
     <row r="63" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="405" t="s">
+      <c r="A63" s="397" t="s">
         <v>87</v>
       </c>
-      <c r="B63" s="405"/>
-      <c r="C63" s="405"/>
-      <c r="D63" s="405"/>
-      <c r="E63" s="405"/>
-      <c r="F63" s="405"/>
-      <c r="G63" s="405"/>
-      <c r="H63" s="405"/>
-      <c r="I63" s="405"/>
-      <c r="J63" s="405"/>
+      <c r="B63" s="397"/>
+      <c r="C63" s="397"/>
+      <c r="D63" s="397"/>
+      <c r="E63" s="397"/>
+      <c r="F63" s="397"/>
+      <c r="G63" s="397"/>
+      <c r="H63" s="397"/>
+      <c r="I63" s="397"/>
+      <c r="J63" s="397"/>
       <c r="K63" s="6"/>
       <c r="L63" s="6"/>
       <c r="M63" s="6"/>
@@ -8381,18 +8381,18 @@
       <c r="P63" s="6"/>
     </row>
     <row r="64" spans="1:16" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="403" t="s">
+      <c r="A64" s="395" t="s">
         <v>88</v>
       </c>
-      <c r="B64" s="403"/>
-      <c r="C64" s="403"/>
-      <c r="D64" s="403"/>
-      <c r="E64" s="403"/>
-      <c r="F64" s="403"/>
-      <c r="G64" s="403"/>
-      <c r="H64" s="403"/>
-      <c r="I64" s="403"/>
-      <c r="J64" s="403"/>
+      <c r="B64" s="395"/>
+      <c r="C64" s="395"/>
+      <c r="D64" s="395"/>
+      <c r="E64" s="395"/>
+      <c r="F64" s="395"/>
+      <c r="G64" s="395"/>
+      <c r="H64" s="395"/>
+      <c r="I64" s="395"/>
+      <c r="J64" s="395"/>
       <c r="K64" s="6"/>
       <c r="L64" s="6"/>
       <c r="M64" s="6"/>
@@ -8401,18 +8401,18 @@
       <c r="P64" s="6"/>
     </row>
     <row r="65" spans="1:19" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="403" t="s">
+      <c r="A65" s="395" t="s">
         <v>89</v>
       </c>
-      <c r="B65" s="403"/>
-      <c r="C65" s="403"/>
-      <c r="D65" s="403"/>
-      <c r="E65" s="403"/>
-      <c r="F65" s="403"/>
-      <c r="G65" s="403"/>
-      <c r="H65" s="403"/>
-      <c r="I65" s="403"/>
-      <c r="J65" s="403"/>
+      <c r="B65" s="395"/>
+      <c r="C65" s="395"/>
+      <c r="D65" s="395"/>
+      <c r="E65" s="395"/>
+      <c r="F65" s="395"/>
+      <c r="G65" s="395"/>
+      <c r="H65" s="395"/>
+      <c r="I65" s="395"/>
+      <c r="J65" s="395"/>
       <c r="K65" s="6"/>
       <c r="L65" s="6"/>
       <c r="M65" s="6"/>
@@ -8421,18 +8421,18 @@
       <c r="P65" s="6"/>
     </row>
     <row r="66" spans="1:19" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="403" t="s">
+      <c r="A66" s="395" t="s">
         <v>90</v>
       </c>
-      <c r="B66" s="403"/>
-      <c r="C66" s="403"/>
-      <c r="D66" s="403"/>
-      <c r="E66" s="403"/>
-      <c r="F66" s="403"/>
-      <c r="G66" s="403"/>
-      <c r="H66" s="403"/>
-      <c r="I66" s="403"/>
-      <c r="J66" s="403"/>
+      <c r="B66" s="395"/>
+      <c r="C66" s="395"/>
+      <c r="D66" s="395"/>
+      <c r="E66" s="395"/>
+      <c r="F66" s="395"/>
+      <c r="G66" s="395"/>
+      <c r="H66" s="395"/>
+      <c r="I66" s="395"/>
+      <c r="J66" s="395"/>
       <c r="K66" s="6"/>
       <c r="L66" s="6"/>
       <c r="M66" s="6"/>
@@ -8441,18 +8441,18 @@
       <c r="P66" s="6"/>
     </row>
     <row r="67" spans="1:19" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="403" t="s">
+      <c r="A67" s="395" t="s">
         <v>91</v>
       </c>
-      <c r="B67" s="403"/>
-      <c r="C67" s="403"/>
-      <c r="D67" s="403"/>
-      <c r="E67" s="403"/>
-      <c r="F67" s="403"/>
-      <c r="G67" s="403"/>
-      <c r="H67" s="403"/>
-      <c r="I67" s="403"/>
-      <c r="J67" s="403"/>
+      <c r="B67" s="395"/>
+      <c r="C67" s="395"/>
+      <c r="D67" s="395"/>
+      <c r="E67" s="395"/>
+      <c r="F67" s="395"/>
+      <c r="G67" s="395"/>
+      <c r="H67" s="395"/>
+      <c r="I67" s="395"/>
+      <c r="J67" s="395"/>
       <c r="K67" s="6"/>
       <c r="L67" s="6"/>
       <c r="M67" s="6"/>
@@ -8461,18 +8461,18 @@
       <c r="P67" s="6"/>
     </row>
     <row r="68" spans="1:19" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="403" t="s">
+      <c r="A68" s="395" t="s">
         <v>92</v>
       </c>
-      <c r="B68" s="403"/>
-      <c r="C68" s="403"/>
-      <c r="D68" s="403"/>
-      <c r="E68" s="403"/>
-      <c r="F68" s="403"/>
-      <c r="G68" s="403"/>
-      <c r="H68" s="403"/>
-      <c r="I68" s="403"/>
-      <c r="J68" s="403"/>
+      <c r="B68" s="395"/>
+      <c r="C68" s="395"/>
+      <c r="D68" s="395"/>
+      <c r="E68" s="395"/>
+      <c r="F68" s="395"/>
+      <c r="G68" s="395"/>
+      <c r="H68" s="395"/>
+      <c r="I68" s="395"/>
+      <c r="J68" s="395"/>
       <c r="K68" s="6"/>
       <c r="L68" s="6"/>
       <c r="M68" s="6"/>
@@ -8481,18 +8481,18 @@
       <c r="P68" s="6"/>
     </row>
     <row r="69" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="404" t="s">
+      <c r="A69" s="396" t="s">
         <v>93</v>
       </c>
-      <c r="B69" s="404"/>
-      <c r="C69" s="404"/>
-      <c r="D69" s="404"/>
-      <c r="E69" s="404"/>
-      <c r="F69" s="404"/>
-      <c r="G69" s="404"/>
-      <c r="H69" s="404"/>
-      <c r="I69" s="404"/>
-      <c r="J69" s="404"/>
+      <c r="B69" s="396"/>
+      <c r="C69" s="396"/>
+      <c r="D69" s="396"/>
+      <c r="E69" s="396"/>
+      <c r="F69" s="396"/>
+      <c r="G69" s="396"/>
+      <c r="H69" s="396"/>
+      <c r="I69" s="396"/>
+      <c r="J69" s="396"/>
       <c r="K69" s="6"/>
       <c r="L69" s="6"/>
       <c r="M69" s="6"/>
@@ -16442,6 +16442,16 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="18">
+    <mergeCell ref="B1:K1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="A11:K11"/>
+    <mergeCell ref="A57:K57"/>
+    <mergeCell ref="A58:K58"/>
+    <mergeCell ref="A61:J61"/>
     <mergeCell ref="A67:J67"/>
     <mergeCell ref="A68:J68"/>
     <mergeCell ref="A69:J69"/>
@@ -16450,16 +16460,6 @@
     <mergeCell ref="A64:J64"/>
     <mergeCell ref="A65:J65"/>
     <mergeCell ref="A66:J66"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="A11:K11"/>
-    <mergeCell ref="A57:K57"/>
-    <mergeCell ref="A58:K58"/>
-    <mergeCell ref="A61:J61"/>
-    <mergeCell ref="B1:K1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C7:F7"/>
   </mergeCells>
   <dataValidations count="15">
     <dataValidation type="list" prompt="Choose from the list." sqref="C15">
@@ -16616,18 +16616,18 @@
   <sheetData>
     <row r="1" spans="1:25" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="23"/>
-      <c r="B1" s="395" t="s">
+      <c r="B1" s="403" t="s">
         <v>128</v>
       </c>
-      <c r="C1" s="395"/>
-      <c r="D1" s="395"/>
-      <c r="E1" s="395"/>
-      <c r="F1" s="395"/>
-      <c r="G1" s="395"/>
-      <c r="H1" s="395"/>
-      <c r="I1" s="395"/>
-      <c r="J1" s="395"/>
-      <c r="K1" s="395"/>
+      <c r="C1" s="403"/>
+      <c r="D1" s="403"/>
+      <c r="E1" s="403"/>
+      <c r="F1" s="403"/>
+      <c r="G1" s="403"/>
+      <c r="H1" s="403"/>
+      <c r="I1" s="403"/>
+      <c r="J1" s="403"/>
+      <c r="K1" s="403"/>
       <c r="L1" s="6" t="s">
         <v>1</v>
       </c>
@@ -16651,19 +16651,19 @@
       </c>
     </row>
     <row r="2" spans="1:25" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="406" t="s">
+      <c r="A2" s="415" t="s">
         <v>129</v>
       </c>
-      <c r="B2" s="406"/>
-      <c r="C2" s="406"/>
-      <c r="D2" s="406"/>
-      <c r="E2" s="406"/>
-      <c r="F2" s="406"/>
-      <c r="G2" s="406"/>
-      <c r="H2" s="406"/>
-      <c r="I2" s="406"/>
-      <c r="J2" s="406"/>
-      <c r="K2" s="406"/>
+      <c r="B2" s="415"/>
+      <c r="C2" s="415"/>
+      <c r="D2" s="415"/>
+      <c r="E2" s="415"/>
+      <c r="F2" s="415"/>
+      <c r="G2" s="415"/>
+      <c r="H2" s="415"/>
+      <c r="I2" s="415"/>
+      <c r="J2" s="415"/>
+      <c r="K2" s="415"/>
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
       <c r="N2" s="6"/>
@@ -16672,20 +16672,20 @@
     </row>
     <row r="3" spans="1:25" s="76" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="75"/>
-      <c r="B3" s="407" t="s">
+      <c r="B3" s="416" t="s">
         <v>130</v>
       </c>
-      <c r="C3" s="407"/>
-      <c r="D3" s="407"/>
-      <c r="E3" s="407"/>
-      <c r="F3" s="407"/>
-      <c r="G3" s="408" t="s">
+      <c r="C3" s="416"/>
+      <c r="D3" s="416"/>
+      <c r="E3" s="416"/>
+      <c r="F3" s="416"/>
+      <c r="G3" s="417" t="s">
         <v>131</v>
       </c>
-      <c r="H3" s="408"/>
-      <c r="I3" s="408"/>
-      <c r="J3" s="408"/>
-      <c r="K3" s="408"/>
+      <c r="H3" s="417"/>
+      <c r="I3" s="417"/>
+      <c r="J3" s="417"/>
+      <c r="K3" s="417"/>
       <c r="L3" s="6"/>
       <c r="M3" s="6"/>
       <c r="N3" s="6"/>
@@ -17620,17 +17620,17 @@
       <c r="R30" s="7"/>
     </row>
     <row r="31" spans="1:25" s="61" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="409"/>
-      <c r="B31" s="409"/>
-      <c r="C31" s="409"/>
-      <c r="D31" s="409"/>
-      <c r="E31" s="409"/>
-      <c r="F31" s="409"/>
-      <c r="G31" s="409"/>
-      <c r="H31" s="409"/>
-      <c r="I31" s="409"/>
-      <c r="J31" s="409"/>
-      <c r="K31" s="409"/>
+      <c r="A31" s="418"/>
+      <c r="B31" s="418"/>
+      <c r="C31" s="418"/>
+      <c r="D31" s="418"/>
+      <c r="E31" s="418"/>
+      <c r="F31" s="418"/>
+      <c r="G31" s="418"/>
+      <c r="H31" s="418"/>
+      <c r="I31" s="418"/>
+      <c r="J31" s="418"/>
+      <c r="K31" s="418"/>
       <c r="L31" s="6"/>
       <c r="M31" s="6"/>
       <c r="N31" s="6"/>
@@ -17718,19 +17718,19 @@
       <c r="R35" s="7"/>
     </row>
     <row r="36" spans="1:18" ht="69" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="410" t="s">
+      <c r="A36" s="412" t="s">
         <v>151</v>
       </c>
-      <c r="B36" s="410"/>
-      <c r="C36" s="410"/>
-      <c r="D36" s="410"/>
-      <c r="E36" s="410"/>
-      <c r="F36" s="410"/>
-      <c r="G36" s="410"/>
-      <c r="H36" s="410"/>
-      <c r="I36" s="410"/>
-      <c r="J36" s="410"/>
-      <c r="K36" s="410"/>
+      <c r="B36" s="412"/>
+      <c r="C36" s="412"/>
+      <c r="D36" s="412"/>
+      <c r="E36" s="412"/>
+      <c r="F36" s="412"/>
+      <c r="G36" s="412"/>
+      <c r="H36" s="412"/>
+      <c r="I36" s="412"/>
+      <c r="J36" s="412"/>
+      <c r="K36" s="412"/>
       <c r="L36" s="6"/>
       <c r="M36" s="6"/>
       <c r="N36" s="6"/>
@@ -17738,19 +17738,19 @@
       <c r="R36" s="7"/>
     </row>
     <row r="37" spans="1:18" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="410" t="s">
+      <c r="A37" s="412" t="s">
         <v>152</v>
       </c>
-      <c r="B37" s="410"/>
-      <c r="C37" s="410"/>
-      <c r="D37" s="410"/>
-      <c r="E37" s="410"/>
-      <c r="F37" s="410"/>
-      <c r="G37" s="410"/>
-      <c r="H37" s="410"/>
-      <c r="I37" s="410"/>
-      <c r="J37" s="410"/>
-      <c r="K37" s="410"/>
+      <c r="B37" s="412"/>
+      <c r="C37" s="412"/>
+      <c r="D37" s="412"/>
+      <c r="E37" s="412"/>
+      <c r="F37" s="412"/>
+      <c r="G37" s="412"/>
+      <c r="H37" s="412"/>
+      <c r="I37" s="412"/>
+      <c r="J37" s="412"/>
+      <c r="K37" s="412"/>
       <c r="L37" s="6"/>
       <c r="M37" s="6"/>
       <c r="N37" s="6"/>
@@ -17796,55 +17796,55 @@
       <c r="N39" s="6"/>
     </row>
     <row r="40" spans="1:18" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="412" t="s">
+      <c r="A40" s="414" t="s">
         <v>155</v>
       </c>
-      <c r="B40" s="412"/>
-      <c r="C40" s="412"/>
-      <c r="D40" s="412"/>
-      <c r="E40" s="412"/>
-      <c r="F40" s="412"/>
-      <c r="G40" s="412"/>
-      <c r="H40" s="412"/>
-      <c r="I40" s="412"/>
-      <c r="J40" s="412"/>
-      <c r="K40" s="412"/>
+      <c r="B40" s="414"/>
+      <c r="C40" s="414"/>
+      <c r="D40" s="414"/>
+      <c r="E40" s="414"/>
+      <c r="F40" s="414"/>
+      <c r="G40" s="414"/>
+      <c r="H40" s="414"/>
+      <c r="I40" s="414"/>
+      <c r="J40" s="414"/>
+      <c r="K40" s="414"/>
       <c r="L40" s="6"/>
       <c r="M40" s="6"/>
       <c r="N40" s="6"/>
     </row>
     <row r="41" spans="1:18" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="413" t="s">
+      <c r="A41" s="410" t="s">
         <v>156</v>
       </c>
-      <c r="B41" s="413"/>
-      <c r="C41" s="413"/>
-      <c r="D41" s="413"/>
-      <c r="E41" s="413"/>
-      <c r="F41" s="413"/>
-      <c r="G41" s="413"/>
-      <c r="H41" s="413"/>
-      <c r="I41" s="413"/>
-      <c r="J41" s="413"/>
-      <c r="K41" s="413"/>
+      <c r="B41" s="410"/>
+      <c r="C41" s="410"/>
+      <c r="D41" s="410"/>
+      <c r="E41" s="410"/>
+      <c r="F41" s="410"/>
+      <c r="G41" s="410"/>
+      <c r="H41" s="410"/>
+      <c r="I41" s="410"/>
+      <c r="J41" s="410"/>
+      <c r="K41" s="410"/>
       <c r="L41" s="6"/>
       <c r="M41" s="6"/>
       <c r="N41" s="6"/>
     </row>
     <row r="42" spans="1:18" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="413" t="s">
+      <c r="A42" s="410" t="s">
         <v>157</v>
       </c>
-      <c r="B42" s="413"/>
-      <c r="C42" s="413"/>
-      <c r="D42" s="413"/>
-      <c r="E42" s="413"/>
-      <c r="F42" s="413"/>
-      <c r="G42" s="413"/>
-      <c r="H42" s="413"/>
-      <c r="I42" s="413"/>
-      <c r="J42" s="413"/>
-      <c r="K42" s="413"/>
+      <c r="B42" s="410"/>
+      <c r="C42" s="410"/>
+      <c r="D42" s="410"/>
+      <c r="E42" s="410"/>
+      <c r="F42" s="410"/>
+      <c r="G42" s="410"/>
+      <c r="H42" s="410"/>
+      <c r="I42" s="410"/>
+      <c r="J42" s="410"/>
+      <c r="K42" s="410"/>
       <c r="L42" s="6"/>
       <c r="M42" s="6"/>
       <c r="N42" s="6"/>
@@ -17868,19 +17868,19 @@
       <c r="N43" s="6"/>
     </row>
     <row r="44" spans="1:18" ht="126.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="410" t="s">
+      <c r="A44" s="412" t="s">
         <v>159</v>
       </c>
-      <c r="B44" s="410"/>
-      <c r="C44" s="410"/>
-      <c r="D44" s="410"/>
-      <c r="E44" s="410"/>
-      <c r="F44" s="410"/>
-      <c r="G44" s="410"/>
-      <c r="H44" s="410"/>
-      <c r="I44" s="410"/>
-      <c r="J44" s="410"/>
-      <c r="K44" s="410"/>
+      <c r="B44" s="412"/>
+      <c r="C44" s="412"/>
+      <c r="D44" s="412"/>
+      <c r="E44" s="412"/>
+      <c r="F44" s="412"/>
+      <c r="G44" s="412"/>
+      <c r="H44" s="412"/>
+      <c r="I44" s="412"/>
+      <c r="J44" s="412"/>
+      <c r="K44" s="412"/>
       <c r="L44" s="6"/>
       <c r="M44" s="6"/>
       <c r="N44" s="6"/>
@@ -17920,11 +17920,11 @@
       <c r="N46" s="6"/>
     </row>
     <row r="47" spans="1:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="414" t="s">
+      <c r="A47" s="413" t="s">
         <v>161</v>
       </c>
-      <c r="B47" s="414"/>
-      <c r="C47" s="414"/>
+      <c r="B47" s="413"/>
+      <c r="C47" s="413"/>
       <c r="D47" s="109" t="s">
         <v>162</v>
       </c>
@@ -17942,11 +17942,11 @@
       <c r="N47" s="6"/>
     </row>
     <row r="48" spans="1:18" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="415" t="s">
+      <c r="A48" s="408" t="s">
         <v>164</v>
       </c>
-      <c r="B48" s="415"/>
-      <c r="C48" s="415"/>
+      <c r="B48" s="408"/>
+      <c r="C48" s="408"/>
       <c r="D48" s="110" t="s">
         <v>165</v>
       </c>
@@ -17964,11 +17964,11 @@
       <c r="N48" s="6"/>
     </row>
     <row r="49" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="416" t="s">
+      <c r="A49" s="407" t="s">
         <v>166</v>
       </c>
-      <c r="B49" s="416"/>
-      <c r="C49" s="416"/>
+      <c r="B49" s="407"/>
+      <c r="C49" s="407"/>
       <c r="D49" s="111" t="s">
         <v>167</v>
       </c>
@@ -17986,11 +17986,11 @@
       <c r="N49" s="6"/>
     </row>
     <row r="50" spans="1:14" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="415" t="s">
+      <c r="A50" s="408" t="s">
         <v>168</v>
       </c>
-      <c r="B50" s="415"/>
-      <c r="C50" s="415"/>
+      <c r="B50" s="408"/>
+      <c r="C50" s="408"/>
       <c r="D50" s="110" t="s">
         <v>165</v>
       </c>
@@ -18008,11 +18008,11 @@
       <c r="N50" s="6"/>
     </row>
     <row r="51" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="416" t="s">
+      <c r="A51" s="407" t="s">
         <v>169</v>
       </c>
-      <c r="B51" s="416"/>
-      <c r="C51" s="416"/>
+      <c r="B51" s="407"/>
+      <c r="C51" s="407"/>
       <c r="D51" s="111" t="s">
         <v>165</v>
       </c>
@@ -18030,11 +18030,11 @@
       <c r="N51" s="6"/>
     </row>
     <row r="52" spans="1:14" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="415" t="s">
+      <c r="A52" s="408" t="s">
         <v>170</v>
       </c>
-      <c r="B52" s="415"/>
-      <c r="C52" s="415"/>
+      <c r="B52" s="408"/>
+      <c r="C52" s="408"/>
       <c r="D52" s="110" t="s">
         <v>165</v>
       </c>
@@ -18052,11 +18052,11 @@
       <c r="N52" s="6"/>
     </row>
     <row r="53" spans="1:14" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="416" t="s">
+      <c r="A53" s="407" t="s">
         <v>171</v>
       </c>
-      <c r="B53" s="416"/>
-      <c r="C53" s="416"/>
+      <c r="B53" s="407"/>
+      <c r="C53" s="407"/>
       <c r="D53" s="111" t="s">
         <v>165</v>
       </c>
@@ -18074,11 +18074,11 @@
       <c r="N53" s="6"/>
     </row>
     <row r="54" spans="1:14" ht="115.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="415" t="s">
+      <c r="A54" s="408" t="s">
         <v>172</v>
       </c>
-      <c r="B54" s="415"/>
-      <c r="C54" s="415"/>
+      <c r="B54" s="408"/>
+      <c r="C54" s="408"/>
       <c r="D54" s="110" t="s">
         <v>165</v>
       </c>
@@ -18096,11 +18096,11 @@
       <c r="N54" s="6"/>
     </row>
     <row r="55" spans="1:14" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="416" t="s">
+      <c r="A55" s="407" t="s">
         <v>173</v>
       </c>
-      <c r="B55" s="416"/>
-      <c r="C55" s="416"/>
+      <c r="B55" s="407"/>
+      <c r="C55" s="407"/>
       <c r="D55" s="111" t="s">
         <v>165</v>
       </c>
@@ -18134,55 +18134,55 @@
       <c r="N56" s="6"/>
     </row>
     <row r="57" spans="1:14" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="418" t="s">
+      <c r="A57" s="409" t="s">
         <v>174</v>
       </c>
-      <c r="B57" s="418"/>
-      <c r="C57" s="418"/>
-      <c r="D57" s="418"/>
-      <c r="E57" s="418"/>
-      <c r="F57" s="418"/>
-      <c r="G57" s="418"/>
-      <c r="H57" s="418"/>
-      <c r="I57" s="418"/>
-      <c r="J57" s="418"/>
-      <c r="K57" s="418"/>
+      <c r="B57" s="409"/>
+      <c r="C57" s="409"/>
+      <c r="D57" s="409"/>
+      <c r="E57" s="409"/>
+      <c r="F57" s="409"/>
+      <c r="G57" s="409"/>
+      <c r="H57" s="409"/>
+      <c r="I57" s="409"/>
+      <c r="J57" s="409"/>
+      <c r="K57" s="409"/>
       <c r="L57" s="6"/>
       <c r="M57" s="6"/>
       <c r="N57" s="6"/>
     </row>
     <row r="58" spans="1:14" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="418" t="s">
+      <c r="A58" s="409" t="s">
         <v>175</v>
       </c>
-      <c r="B58" s="418"/>
-      <c r="C58" s="418"/>
-      <c r="D58" s="418"/>
-      <c r="E58" s="418"/>
-      <c r="F58" s="418"/>
-      <c r="G58" s="418"/>
-      <c r="H58" s="418"/>
-      <c r="I58" s="418"/>
-      <c r="J58" s="418"/>
-      <c r="K58" s="418"/>
+      <c r="B58" s="409"/>
+      <c r="C58" s="409"/>
+      <c r="D58" s="409"/>
+      <c r="E58" s="409"/>
+      <c r="F58" s="409"/>
+      <c r="G58" s="409"/>
+      <c r="H58" s="409"/>
+      <c r="I58" s="409"/>
+      <c r="J58" s="409"/>
+      <c r="K58" s="409"/>
       <c r="L58" s="6"/>
       <c r="M58" s="6"/>
       <c r="N58" s="6"/>
     </row>
     <row r="59" spans="1:14" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="417" t="s">
+      <c r="A59" s="406" t="s">
         <v>176</v>
       </c>
-      <c r="B59" s="417"/>
-      <c r="C59" s="417"/>
-      <c r="D59" s="417"/>
-      <c r="E59" s="417"/>
-      <c r="F59" s="417"/>
-      <c r="G59" s="417"/>
-      <c r="H59" s="417"/>
-      <c r="I59" s="417"/>
-      <c r="J59" s="417"/>
-      <c r="K59" s="417"/>
+      <c r="B59" s="406"/>
+      <c r="C59" s="406"/>
+      <c r="D59" s="406"/>
+      <c r="E59" s="406"/>
+      <c r="F59" s="406"/>
+      <c r="G59" s="406"/>
+      <c r="H59" s="406"/>
+      <c r="I59" s="406"/>
+      <c r="J59" s="406"/>
+      <c r="K59" s="406"/>
       <c r="L59" s="6"/>
       <c r="M59" s="6"/>
       <c r="N59" s="6"/>
@@ -25309,32 +25309,32 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="26">
+    <mergeCell ref="B1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="G3:K3"/>
+    <mergeCell ref="A31:K31"/>
+    <mergeCell ref="A36:K36"/>
+    <mergeCell ref="A37:K37"/>
+    <mergeCell ref="A38:K38"/>
+    <mergeCell ref="A39:K39"/>
+    <mergeCell ref="A40:K40"/>
+    <mergeCell ref="A41:K41"/>
+    <mergeCell ref="A42:K42"/>
+    <mergeCell ref="A43:K43"/>
+    <mergeCell ref="A44:K44"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="A49:C49"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="A51:C51"/>
+    <mergeCell ref="A52:C52"/>
     <mergeCell ref="A59:K59"/>
     <mergeCell ref="A53:C53"/>
     <mergeCell ref="A54:C54"/>
     <mergeCell ref="A55:C55"/>
     <mergeCell ref="A57:K57"/>
     <mergeCell ref="A58:K58"/>
-    <mergeCell ref="A48:C48"/>
-    <mergeCell ref="A49:C49"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="A51:C51"/>
-    <mergeCell ref="A52:C52"/>
-    <mergeCell ref="A41:K41"/>
-    <mergeCell ref="A42:K42"/>
-    <mergeCell ref="A43:K43"/>
-    <mergeCell ref="A44:K44"/>
-    <mergeCell ref="A47:C47"/>
-    <mergeCell ref="A36:K36"/>
-    <mergeCell ref="A37:K37"/>
-    <mergeCell ref="A38:K38"/>
-    <mergeCell ref="A39:K39"/>
-    <mergeCell ref="A40:K40"/>
-    <mergeCell ref="B1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="G3:K3"/>
-    <mergeCell ref="A31:K31"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A32" r:id="rId1"/>
@@ -25355,7 +25355,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK68"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R38" sqref="R38"/>
     </sheetView>
   </sheetViews>
@@ -25500,25 +25500,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="419" t="s">
+      <c r="A1" s="424" t="s">
         <v>177</v>
       </c>
-      <c r="B1" s="419"/>
-      <c r="C1" s="419"/>
-      <c r="D1" s="419"/>
-      <c r="E1" s="419"/>
-      <c r="F1" s="419"/>
-      <c r="G1" s="419"/>
-      <c r="H1" s="419"/>
-      <c r="I1" s="419"/>
-      <c r="J1" s="419"/>
-      <c r="K1" s="419"/>
-      <c r="L1" s="419"/>
-      <c r="M1" s="419"/>
-      <c r="N1" s="419"/>
-      <c r="O1" s="419"/>
-      <c r="P1" s="419"/>
-      <c r="Q1" s="419"/>
+      <c r="B1" s="424"/>
+      <c r="C1" s="424"/>
+      <c r="D1" s="424"/>
+      <c r="E1" s="424"/>
+      <c r="F1" s="424"/>
+      <c r="G1" s="424"/>
+      <c r="H1" s="424"/>
+      <c r="I1" s="424"/>
+      <c r="J1" s="424"/>
+      <c r="K1" s="424"/>
+      <c r="L1" s="424"/>
+      <c r="M1" s="424"/>
+      <c r="N1" s="424"/>
+      <c r="O1" s="424"/>
+      <c r="P1" s="424"/>
+      <c r="Q1" s="424"/>
       <c r="R1" s="6"/>
       <c r="S1" s="6"/>
       <c r="T1" s="114"/>
@@ -25541,26 +25541,26 @@
     </row>
     <row r="2" spans="1:36" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="116"/>
-      <c r="B2" s="420" t="s">
+      <c r="B2" s="425" t="s">
         <v>178</v>
       </c>
-      <c r="C2" s="420"/>
-      <c r="D2" s="420"/>
-      <c r="E2" s="420"/>
-      <c r="F2" s="420"/>
-      <c r="G2" s="420"/>
-      <c r="H2" s="420"/>
-      <c r="I2" s="420"/>
-      <c r="J2" s="420"/>
-      <c r="K2" s="420"/>
-      <c r="L2" s="420"/>
-      <c r="M2" s="420"/>
+      <c r="C2" s="425"/>
+      <c r="D2" s="425"/>
+      <c r="E2" s="425"/>
+      <c r="F2" s="425"/>
+      <c r="G2" s="425"/>
+      <c r="H2" s="425"/>
+      <c r="I2" s="425"/>
+      <c r="J2" s="425"/>
+      <c r="K2" s="425"/>
+      <c r="L2" s="425"/>
+      <c r="M2" s="425"/>
       <c r="N2" s="24"/>
       <c r="O2" s="24"/>
-      <c r="P2" s="421" t="s">
+      <c r="P2" s="426" t="s">
         <v>179</v>
       </c>
-      <c r="Q2" s="421"/>
+      <c r="Q2" s="426"/>
       <c r="R2" s="117"/>
       <c r="S2" s="6"/>
       <c r="T2" s="114"/>
@@ -25583,36 +25583,36 @@
     </row>
     <row r="3" spans="1:36" s="7" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="118"/>
-      <c r="B3" s="422" t="s">
+      <c r="B3" s="427" t="s">
         <v>180</v>
       </c>
-      <c r="C3" s="422"/>
-      <c r="D3" s="423" t="s">
+      <c r="C3" s="427"/>
+      <c r="D3" s="428" t="s">
         <v>181</v>
       </c>
-      <c r="E3" s="423"/>
-      <c r="F3" s="424" t="s">
+      <c r="E3" s="428"/>
+      <c r="F3" s="429" t="s">
         <v>182</v>
       </c>
-      <c r="G3" s="424"/>
-      <c r="H3" s="423" t="s">
+      <c r="G3" s="429"/>
+      <c r="H3" s="428" t="s">
         <v>183</v>
       </c>
-      <c r="I3" s="423"/>
-      <c r="J3" s="424" t="s">
+      <c r="I3" s="428"/>
+      <c r="J3" s="429" t="s">
         <v>184</v>
       </c>
-      <c r="K3" s="424"/>
-      <c r="L3" s="425" t="s">
+      <c r="K3" s="429"/>
+      <c r="L3" s="430" t="s">
         <v>185</v>
       </c>
-      <c r="M3" s="425"/>
-      <c r="N3" s="426" t="s">
+      <c r="M3" s="430"/>
+      <c r="N3" s="431" t="s">
         <v>186</v>
       </c>
-      <c r="O3" s="426"/>
-      <c r="P3" s="421"/>
-      <c r="Q3" s="421"/>
+      <c r="O3" s="431"/>
+      <c r="P3" s="426"/>
+      <c r="Q3" s="426"/>
       <c r="R3" s="117"/>
       <c r="S3" s="6"/>
       <c r="T3" s="114"/>
@@ -25686,27 +25686,27 @@
         <v>189</v>
       </c>
       <c r="R4" s="117"/>
-      <c r="S4" s="427" t="s">
+      <c r="S4" s="420" t="s">
         <v>190</v>
       </c>
-      <c r="T4" s="427"/>
-      <c r="U4" s="427"/>
-      <c r="V4" s="427"/>
-      <c r="W4" s="427"/>
-      <c r="X4" s="427"/>
-      <c r="Y4" s="427"/>
-      <c r="Z4" s="427"/>
+      <c r="T4" s="420"/>
+      <c r="U4" s="420"/>
+      <c r="V4" s="420"/>
+      <c r="W4" s="420"/>
+      <c r="X4" s="420"/>
+      <c r="Y4" s="420"/>
+      <c r="Z4" s="420"/>
       <c r="AA4" s="6"/>
-      <c r="AB4" s="427" t="s">
+      <c r="AB4" s="420" t="s">
         <v>191</v>
       </c>
-      <c r="AC4" s="427"/>
-      <c r="AD4" s="427"/>
-      <c r="AE4" s="427"/>
-      <c r="AF4" s="427"/>
-      <c r="AG4" s="427"/>
-      <c r="AH4" s="427"/>
-      <c r="AI4" s="427"/>
+      <c r="AC4" s="420"/>
+      <c r="AD4" s="420"/>
+      <c r="AE4" s="420"/>
+      <c r="AF4" s="420"/>
+      <c r="AG4" s="420"/>
+      <c r="AH4" s="420"/>
+      <c r="AI4" s="420"/>
       <c r="AJ4" s="6"/>
     </row>
     <row r="5" spans="1:36" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -30012,25 +30012,25 @@
       <c r="AJ48" s="6"/>
     </row>
     <row r="49" spans="1:36" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="428" t="s">
+      <c r="A49" s="421" t="s">
         <v>218</v>
       </c>
-      <c r="B49" s="428"/>
-      <c r="C49" s="428"/>
-      <c r="D49" s="428"/>
-      <c r="E49" s="428"/>
-      <c r="F49" s="428"/>
-      <c r="G49" s="428"/>
-      <c r="H49" s="428"/>
-      <c r="I49" s="428"/>
-      <c r="J49" s="428"/>
-      <c r="K49" s="428"/>
-      <c r="L49" s="428"/>
-      <c r="M49" s="428"/>
-      <c r="N49" s="428"/>
-      <c r="O49" s="428"/>
-      <c r="P49" s="428"/>
-      <c r="Q49" s="428"/>
+      <c r="B49" s="421"/>
+      <c r="C49" s="421"/>
+      <c r="D49" s="421"/>
+      <c r="E49" s="421"/>
+      <c r="F49" s="421"/>
+      <c r="G49" s="421"/>
+      <c r="H49" s="421"/>
+      <c r="I49" s="421"/>
+      <c r="J49" s="421"/>
+      <c r="K49" s="421"/>
+      <c r="L49" s="421"/>
+      <c r="M49" s="421"/>
+      <c r="N49" s="421"/>
+      <c r="O49" s="421"/>
+      <c r="P49" s="421"/>
+      <c r="Q49" s="421"/>
       <c r="R49" s="6"/>
       <c r="S49" s="6"/>
       <c r="T49" s="114"/>
@@ -30090,25 +30090,25 @@
       <c r="AJ50" s="6"/>
     </row>
     <row r="51" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="429" t="s">
+      <c r="A51" s="422" t="s">
         <v>219</v>
       </c>
-      <c r="B51" s="429"/>
-      <c r="C51" s="429"/>
-      <c r="D51" s="429"/>
-      <c r="E51" s="429"/>
-      <c r="F51" s="429"/>
-      <c r="G51" s="429"/>
-      <c r="H51" s="429"/>
-      <c r="I51" s="429"/>
-      <c r="J51" s="429"/>
-      <c r="K51" s="429"/>
-      <c r="L51" s="429"/>
-      <c r="M51" s="429"/>
-      <c r="N51" s="429"/>
-      <c r="O51" s="429"/>
-      <c r="P51" s="429"/>
-      <c r="Q51" s="429"/>
+      <c r="B51" s="422"/>
+      <c r="C51" s="422"/>
+      <c r="D51" s="422"/>
+      <c r="E51" s="422"/>
+      <c r="F51" s="422"/>
+      <c r="G51" s="422"/>
+      <c r="H51" s="422"/>
+      <c r="I51" s="422"/>
+      <c r="J51" s="422"/>
+      <c r="K51" s="422"/>
+      <c r="L51" s="422"/>
+      <c r="M51" s="422"/>
+      <c r="N51" s="422"/>
+      <c r="O51" s="422"/>
+      <c r="P51" s="422"/>
+      <c r="Q51" s="422"/>
       <c r="R51" s="6"/>
       <c r="S51" s="6"/>
       <c r="T51" s="114"/>
@@ -30130,25 +30130,25 @@
       <c r="AJ51" s="6"/>
     </row>
     <row r="52" spans="1:36" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="430" t="s">
+      <c r="A52" s="423" t="s">
         <v>220</v>
       </c>
-      <c r="B52" s="430"/>
-      <c r="C52" s="430"/>
-      <c r="D52" s="430"/>
-      <c r="E52" s="430"/>
-      <c r="F52" s="430"/>
-      <c r="G52" s="430"/>
-      <c r="H52" s="430"/>
-      <c r="I52" s="430"/>
-      <c r="J52" s="430"/>
-      <c r="K52" s="430"/>
-      <c r="L52" s="430"/>
-      <c r="M52" s="430"/>
-      <c r="N52" s="430"/>
-      <c r="O52" s="430"/>
-      <c r="P52" s="430"/>
-      <c r="Q52" s="430"/>
+      <c r="B52" s="423"/>
+      <c r="C52" s="423"/>
+      <c r="D52" s="423"/>
+      <c r="E52" s="423"/>
+      <c r="F52" s="423"/>
+      <c r="G52" s="423"/>
+      <c r="H52" s="423"/>
+      <c r="I52" s="423"/>
+      <c r="J52" s="423"/>
+      <c r="K52" s="423"/>
+      <c r="L52" s="423"/>
+      <c r="M52" s="423"/>
+      <c r="N52" s="423"/>
+      <c r="O52" s="423"/>
+      <c r="P52" s="423"/>
+      <c r="Q52" s="423"/>
       <c r="R52" s="6"/>
       <c r="S52" s="6"/>
       <c r="T52" s="114"/>
@@ -30169,25 +30169,25 @@
       <c r="AI52" s="115"/>
     </row>
     <row r="53" spans="1:36" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="431" t="s">
+      <c r="A53" s="419" t="s">
         <v>221</v>
       </c>
-      <c r="B53" s="431"/>
-      <c r="C53" s="431"/>
-      <c r="D53" s="431"/>
-      <c r="E53" s="431"/>
-      <c r="F53" s="431"/>
-      <c r="G53" s="431"/>
-      <c r="H53" s="431"/>
-      <c r="I53" s="431"/>
-      <c r="J53" s="431"/>
-      <c r="K53" s="431"/>
-      <c r="L53" s="431"/>
-      <c r="M53" s="431"/>
-      <c r="N53" s="431"/>
-      <c r="O53" s="431"/>
-      <c r="P53" s="431"/>
-      <c r="Q53" s="431"/>
+      <c r="B53" s="419"/>
+      <c r="C53" s="419"/>
+      <c r="D53" s="419"/>
+      <c r="E53" s="419"/>
+      <c r="F53" s="419"/>
+      <c r="G53" s="419"/>
+      <c r="H53" s="419"/>
+      <c r="I53" s="419"/>
+      <c r="J53" s="419"/>
+      <c r="K53" s="419"/>
+      <c r="L53" s="419"/>
+      <c r="M53" s="419"/>
+      <c r="N53" s="419"/>
+      <c r="O53" s="419"/>
+      <c r="P53" s="419"/>
+      <c r="Q53" s="419"/>
       <c r="R53" s="6"/>
       <c r="S53" s="6"/>
       <c r="T53" s="114"/>
@@ -30208,25 +30208,25 @@
       <c r="AI53" s="115"/>
     </row>
     <row r="54" spans="1:36" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="418" t="s">
+      <c r="A54" s="409" t="s">
         <v>222</v>
       </c>
-      <c r="B54" s="418"/>
-      <c r="C54" s="418"/>
-      <c r="D54" s="418"/>
-      <c r="E54" s="418"/>
-      <c r="F54" s="418"/>
-      <c r="G54" s="418"/>
-      <c r="H54" s="418"/>
-      <c r="I54" s="418"/>
-      <c r="J54" s="418"/>
-      <c r="K54" s="418"/>
-      <c r="L54" s="418"/>
-      <c r="M54" s="418"/>
-      <c r="N54" s="418"/>
-      <c r="O54" s="418"/>
-      <c r="P54" s="418"/>
-      <c r="Q54" s="418"/>
+      <c r="B54" s="409"/>
+      <c r="C54" s="409"/>
+      <c r="D54" s="409"/>
+      <c r="E54" s="409"/>
+      <c r="F54" s="409"/>
+      <c r="G54" s="409"/>
+      <c r="H54" s="409"/>
+      <c r="I54" s="409"/>
+      <c r="J54" s="409"/>
+      <c r="K54" s="409"/>
+      <c r="L54" s="409"/>
+      <c r="M54" s="409"/>
+      <c r="N54" s="409"/>
+      <c r="O54" s="409"/>
+      <c r="P54" s="409"/>
+      <c r="Q54" s="409"/>
       <c r="R54" s="6"/>
       <c r="S54" s="6"/>
       <c r="T54" s="114"/>
@@ -30247,25 +30247,25 @@
       <c r="AI54" s="115"/>
     </row>
     <row r="55" spans="1:36" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="418" t="s">
+      <c r="A55" s="409" t="s">
         <v>223</v>
       </c>
-      <c r="B55" s="418"/>
-      <c r="C55" s="418"/>
-      <c r="D55" s="418"/>
-      <c r="E55" s="418"/>
-      <c r="F55" s="418"/>
-      <c r="G55" s="418"/>
-      <c r="H55" s="418"/>
-      <c r="I55" s="418"/>
-      <c r="J55" s="418"/>
-      <c r="K55" s="418"/>
-      <c r="L55" s="418"/>
-      <c r="M55" s="418"/>
-      <c r="N55" s="418"/>
-      <c r="O55" s="418"/>
-      <c r="P55" s="418"/>
-      <c r="Q55" s="418"/>
+      <c r="B55" s="409"/>
+      <c r="C55" s="409"/>
+      <c r="D55" s="409"/>
+      <c r="E55" s="409"/>
+      <c r="F55" s="409"/>
+      <c r="G55" s="409"/>
+      <c r="H55" s="409"/>
+      <c r="I55" s="409"/>
+      <c r="J55" s="409"/>
+      <c r="K55" s="409"/>
+      <c r="L55" s="409"/>
+      <c r="M55" s="409"/>
+      <c r="N55" s="409"/>
+      <c r="O55" s="409"/>
+      <c r="P55" s="409"/>
+      <c r="Q55" s="409"/>
       <c r="R55" s="6"/>
       <c r="S55" s="6"/>
       <c r="T55" s="114"/>
@@ -30286,25 +30286,25 @@
       <c r="AI55" s="115"/>
     </row>
     <row r="56" spans="1:36" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="418" t="s">
+      <c r="A56" s="409" t="s">
         <v>224</v>
       </c>
-      <c r="B56" s="418"/>
-      <c r="C56" s="418"/>
-      <c r="D56" s="418"/>
-      <c r="E56" s="418"/>
-      <c r="F56" s="418"/>
-      <c r="G56" s="418"/>
-      <c r="H56" s="418"/>
-      <c r="I56" s="418"/>
-      <c r="J56" s="418"/>
-      <c r="K56" s="418"/>
-      <c r="L56" s="418"/>
-      <c r="M56" s="418"/>
-      <c r="N56" s="418"/>
-      <c r="O56" s="418"/>
-      <c r="P56" s="418"/>
-      <c r="Q56" s="418"/>
+      <c r="B56" s="409"/>
+      <c r="C56" s="409"/>
+      <c r="D56" s="409"/>
+      <c r="E56" s="409"/>
+      <c r="F56" s="409"/>
+      <c r="G56" s="409"/>
+      <c r="H56" s="409"/>
+      <c r="I56" s="409"/>
+      <c r="J56" s="409"/>
+      <c r="K56" s="409"/>
+      <c r="L56" s="409"/>
+      <c r="M56" s="409"/>
+      <c r="N56" s="409"/>
+      <c r="O56" s="409"/>
+      <c r="P56" s="409"/>
+      <c r="Q56" s="409"/>
       <c r="R56" s="6"/>
       <c r="S56" s="6"/>
       <c r="T56" s="114"/>
@@ -30325,25 +30325,25 @@
       <c r="AI56" s="115"/>
     </row>
     <row r="57" spans="1:36" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="418" t="s">
+      <c r="A57" s="409" t="s">
         <v>225</v>
       </c>
-      <c r="B57" s="418"/>
-      <c r="C57" s="418"/>
-      <c r="D57" s="418"/>
-      <c r="E57" s="418"/>
-      <c r="F57" s="418"/>
-      <c r="G57" s="418"/>
-      <c r="H57" s="418"/>
-      <c r="I57" s="418"/>
-      <c r="J57" s="418"/>
-      <c r="K57" s="418"/>
-      <c r="L57" s="418"/>
-      <c r="M57" s="418"/>
-      <c r="N57" s="418"/>
-      <c r="O57" s="418"/>
-      <c r="P57" s="418"/>
-      <c r="Q57" s="418"/>
+      <c r="B57" s="409"/>
+      <c r="C57" s="409"/>
+      <c r="D57" s="409"/>
+      <c r="E57" s="409"/>
+      <c r="F57" s="409"/>
+      <c r="G57" s="409"/>
+      <c r="H57" s="409"/>
+      <c r="I57" s="409"/>
+      <c r="J57" s="409"/>
+      <c r="K57" s="409"/>
+      <c r="L57" s="409"/>
+      <c r="M57" s="409"/>
+      <c r="N57" s="409"/>
+      <c r="O57" s="409"/>
+      <c r="P57" s="409"/>
+      <c r="Q57" s="409"/>
       <c r="R57" s="6"/>
       <c r="S57" s="6"/>
       <c r="T57" s="114"/>
@@ -30364,25 +30364,25 @@
       <c r="AI57" s="115"/>
     </row>
     <row r="58" spans="1:36" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="418" t="s">
+      <c r="A58" s="409" t="s">
         <v>226</v>
       </c>
-      <c r="B58" s="418"/>
-      <c r="C58" s="418"/>
-      <c r="D58" s="418"/>
-      <c r="E58" s="418"/>
-      <c r="F58" s="418"/>
-      <c r="G58" s="418"/>
-      <c r="H58" s="418"/>
-      <c r="I58" s="418"/>
-      <c r="J58" s="418"/>
-      <c r="K58" s="418"/>
-      <c r="L58" s="418"/>
-      <c r="M58" s="418"/>
-      <c r="N58" s="418"/>
-      <c r="O58" s="418"/>
-      <c r="P58" s="418"/>
-      <c r="Q58" s="418"/>
+      <c r="B58" s="409"/>
+      <c r="C58" s="409"/>
+      <c r="D58" s="409"/>
+      <c r="E58" s="409"/>
+      <c r="F58" s="409"/>
+      <c r="G58" s="409"/>
+      <c r="H58" s="409"/>
+      <c r="I58" s="409"/>
+      <c r="J58" s="409"/>
+      <c r="K58" s="409"/>
+      <c r="L58" s="409"/>
+      <c r="M58" s="409"/>
+      <c r="N58" s="409"/>
+      <c r="O58" s="409"/>
+      <c r="P58" s="409"/>
+      <c r="Q58" s="409"/>
       <c r="R58" s="6"/>
       <c r="S58" s="6"/>
       <c r="T58" s="114"/>
@@ -30403,25 +30403,25 @@
       <c r="AI58" s="115"/>
     </row>
     <row r="59" spans="1:36" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="418" t="s">
+      <c r="A59" s="409" t="s">
         <v>227</v>
       </c>
-      <c r="B59" s="418"/>
-      <c r="C59" s="418"/>
-      <c r="D59" s="418"/>
-      <c r="E59" s="418"/>
-      <c r="F59" s="418"/>
-      <c r="G59" s="418"/>
-      <c r="H59" s="418"/>
-      <c r="I59" s="418"/>
-      <c r="J59" s="418"/>
-      <c r="K59" s="418"/>
-      <c r="L59" s="418"/>
-      <c r="M59" s="418"/>
-      <c r="N59" s="418"/>
-      <c r="O59" s="418"/>
-      <c r="P59" s="418"/>
-      <c r="Q59" s="418"/>
+      <c r="B59" s="409"/>
+      <c r="C59" s="409"/>
+      <c r="D59" s="409"/>
+      <c r="E59" s="409"/>
+      <c r="F59" s="409"/>
+      <c r="G59" s="409"/>
+      <c r="H59" s="409"/>
+      <c r="I59" s="409"/>
+      <c r="J59" s="409"/>
+      <c r="K59" s="409"/>
+      <c r="L59" s="409"/>
+      <c r="M59" s="409"/>
+      <c r="N59" s="409"/>
+      <c r="O59" s="409"/>
+      <c r="P59" s="409"/>
+      <c r="Q59" s="409"/>
       <c r="R59" s="6"/>
       <c r="S59" s="6"/>
       <c r="T59" s="114"/>
@@ -30442,25 +30442,25 @@
       <c r="AI59" s="115"/>
     </row>
     <row r="60" spans="1:36" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="418" t="s">
+      <c r="A60" s="409" t="s">
         <v>228</v>
       </c>
-      <c r="B60" s="418"/>
-      <c r="C60" s="418"/>
-      <c r="D60" s="418"/>
-      <c r="E60" s="418"/>
-      <c r="F60" s="418"/>
-      <c r="G60" s="418"/>
-      <c r="H60" s="418"/>
-      <c r="I60" s="418"/>
-      <c r="J60" s="418"/>
-      <c r="K60" s="418"/>
-      <c r="L60" s="418"/>
-      <c r="M60" s="418"/>
-      <c r="N60" s="418"/>
-      <c r="O60" s="418"/>
-      <c r="P60" s="418"/>
-      <c r="Q60" s="418"/>
+      <c r="B60" s="409"/>
+      <c r="C60" s="409"/>
+      <c r="D60" s="409"/>
+      <c r="E60" s="409"/>
+      <c r="F60" s="409"/>
+      <c r="G60" s="409"/>
+      <c r="H60" s="409"/>
+      <c r="I60" s="409"/>
+      <c r="J60" s="409"/>
+      <c r="K60" s="409"/>
+      <c r="L60" s="409"/>
+      <c r="M60" s="409"/>
+      <c r="N60" s="409"/>
+      <c r="O60" s="409"/>
+      <c r="P60" s="409"/>
+      <c r="Q60" s="409"/>
       <c r="R60" s="6"/>
       <c r="S60" s="6"/>
       <c r="T60" s="114"/>
@@ -30481,25 +30481,25 @@
       <c r="AI60" s="115"/>
     </row>
     <row r="61" spans="1:36" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="418" t="s">
+      <c r="A61" s="409" t="s">
         <v>229</v>
       </c>
-      <c r="B61" s="418"/>
-      <c r="C61" s="418"/>
-      <c r="D61" s="418"/>
-      <c r="E61" s="418"/>
-      <c r="F61" s="418"/>
-      <c r="G61" s="418"/>
-      <c r="H61" s="418"/>
-      <c r="I61" s="418"/>
-      <c r="J61" s="418"/>
-      <c r="K61" s="418"/>
-      <c r="L61" s="418"/>
-      <c r="M61" s="418"/>
-      <c r="N61" s="418"/>
-      <c r="O61" s="418"/>
-      <c r="P61" s="418"/>
-      <c r="Q61" s="418"/>
+      <c r="B61" s="409"/>
+      <c r="C61" s="409"/>
+      <c r="D61" s="409"/>
+      <c r="E61" s="409"/>
+      <c r="F61" s="409"/>
+      <c r="G61" s="409"/>
+      <c r="H61" s="409"/>
+      <c r="I61" s="409"/>
+      <c r="J61" s="409"/>
+      <c r="K61" s="409"/>
+      <c r="L61" s="409"/>
+      <c r="M61" s="409"/>
+      <c r="N61" s="409"/>
+      <c r="O61" s="409"/>
+      <c r="P61" s="409"/>
+      <c r="Q61" s="409"/>
       <c r="R61" s="6"/>
       <c r="S61" s="6"/>
       <c r="T61" s="114"/>
@@ -30520,25 +30520,25 @@
       <c r="AI61" s="115"/>
     </row>
     <row r="62" spans="1:36" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="418" t="s">
+      <c r="A62" s="409" t="s">
         <v>230</v>
       </c>
-      <c r="B62" s="418"/>
-      <c r="C62" s="418"/>
-      <c r="D62" s="418"/>
-      <c r="E62" s="418"/>
-      <c r="F62" s="418"/>
-      <c r="G62" s="418"/>
-      <c r="H62" s="418"/>
-      <c r="I62" s="418"/>
-      <c r="J62" s="418"/>
-      <c r="K62" s="418"/>
-      <c r="L62" s="418"/>
-      <c r="M62" s="418"/>
-      <c r="N62" s="418"/>
-      <c r="O62" s="418"/>
-      <c r="P62" s="418"/>
-      <c r="Q62" s="418"/>
+      <c r="B62" s="409"/>
+      <c r="C62" s="409"/>
+      <c r="D62" s="409"/>
+      <c r="E62" s="409"/>
+      <c r="F62" s="409"/>
+      <c r="G62" s="409"/>
+      <c r="H62" s="409"/>
+      <c r="I62" s="409"/>
+      <c r="J62" s="409"/>
+      <c r="K62" s="409"/>
+      <c r="L62" s="409"/>
+      <c r="M62" s="409"/>
+      <c r="N62" s="409"/>
+      <c r="O62" s="409"/>
+      <c r="P62" s="409"/>
+      <c r="Q62" s="409"/>
       <c r="R62" s="6"/>
       <c r="S62" s="6"/>
       <c r="T62" s="114"/>
@@ -30559,25 +30559,25 @@
       <c r="AI62" s="115"/>
     </row>
     <row r="63" spans="1:36" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="418" t="s">
+      <c r="A63" s="409" t="s">
         <v>231</v>
       </c>
-      <c r="B63" s="418"/>
-      <c r="C63" s="418"/>
-      <c r="D63" s="418"/>
-      <c r="E63" s="418"/>
-      <c r="F63" s="418"/>
-      <c r="G63" s="418"/>
-      <c r="H63" s="418"/>
-      <c r="I63" s="418"/>
-      <c r="J63" s="418"/>
-      <c r="K63" s="418"/>
-      <c r="L63" s="418"/>
-      <c r="M63" s="418"/>
-      <c r="N63" s="418"/>
-      <c r="O63" s="418"/>
-      <c r="P63" s="418"/>
-      <c r="Q63" s="418"/>
+      <c r="B63" s="409"/>
+      <c r="C63" s="409"/>
+      <c r="D63" s="409"/>
+      <c r="E63" s="409"/>
+      <c r="F63" s="409"/>
+      <c r="G63" s="409"/>
+      <c r="H63" s="409"/>
+      <c r="I63" s="409"/>
+      <c r="J63" s="409"/>
+      <c r="K63" s="409"/>
+      <c r="L63" s="409"/>
+      <c r="M63" s="409"/>
+      <c r="N63" s="409"/>
+      <c r="O63" s="409"/>
+      <c r="P63" s="409"/>
+      <c r="Q63" s="409"/>
       <c r="R63" s="6"/>
       <c r="S63" s="6"/>
       <c r="T63" s="114"/>
@@ -30598,25 +30598,25 @@
       <c r="AI63" s="115"/>
     </row>
     <row r="64" spans="1:36" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="418" t="s">
+      <c r="A64" s="409" t="s">
         <v>232</v>
       </c>
-      <c r="B64" s="418"/>
-      <c r="C64" s="418"/>
-      <c r="D64" s="418"/>
-      <c r="E64" s="418"/>
-      <c r="F64" s="418"/>
-      <c r="G64" s="418"/>
-      <c r="H64" s="418"/>
-      <c r="I64" s="418"/>
-      <c r="J64" s="418"/>
-      <c r="K64" s="418"/>
-      <c r="L64" s="418"/>
-      <c r="M64" s="418"/>
-      <c r="N64" s="418"/>
-      <c r="O64" s="418"/>
-      <c r="P64" s="418"/>
-      <c r="Q64" s="418"/>
+      <c r="B64" s="409"/>
+      <c r="C64" s="409"/>
+      <c r="D64" s="409"/>
+      <c r="E64" s="409"/>
+      <c r="F64" s="409"/>
+      <c r="G64" s="409"/>
+      <c r="H64" s="409"/>
+      <c r="I64" s="409"/>
+      <c r="J64" s="409"/>
+      <c r="K64" s="409"/>
+      <c r="L64" s="409"/>
+      <c r="M64" s="409"/>
+      <c r="N64" s="409"/>
+      <c r="O64" s="409"/>
+      <c r="P64" s="409"/>
+      <c r="Q64" s="409"/>
       <c r="R64" s="6"/>
       <c r="S64" s="6"/>
       <c r="T64" s="114"/>
@@ -30637,25 +30637,25 @@
       <c r="AI64" s="115"/>
     </row>
     <row r="65" spans="1:35" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="418" t="s">
+      <c r="A65" s="409" t="s">
         <v>233</v>
       </c>
-      <c r="B65" s="418"/>
-      <c r="C65" s="418"/>
-      <c r="D65" s="418"/>
-      <c r="E65" s="418"/>
-      <c r="F65" s="418"/>
-      <c r="G65" s="418"/>
-      <c r="H65" s="418"/>
-      <c r="I65" s="418"/>
-      <c r="J65" s="418"/>
-      <c r="K65" s="418"/>
-      <c r="L65" s="418"/>
-      <c r="M65" s="418"/>
-      <c r="N65" s="418"/>
-      <c r="O65" s="418"/>
-      <c r="P65" s="418"/>
-      <c r="Q65" s="418"/>
+      <c r="B65" s="409"/>
+      <c r="C65" s="409"/>
+      <c r="D65" s="409"/>
+      <c r="E65" s="409"/>
+      <c r="F65" s="409"/>
+      <c r="G65" s="409"/>
+      <c r="H65" s="409"/>
+      <c r="I65" s="409"/>
+      <c r="J65" s="409"/>
+      <c r="K65" s="409"/>
+      <c r="L65" s="409"/>
+      <c r="M65" s="409"/>
+      <c r="N65" s="409"/>
+      <c r="O65" s="409"/>
+      <c r="P65" s="409"/>
+      <c r="Q65" s="409"/>
       <c r="R65" s="6"/>
       <c r="S65" s="6"/>
       <c r="T65" s="114"/>
@@ -30676,25 +30676,25 @@
       <c r="AI65" s="115"/>
     </row>
     <row r="66" spans="1:35" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="418" t="s">
+      <c r="A66" s="409" t="s">
         <v>234</v>
       </c>
-      <c r="B66" s="418"/>
-      <c r="C66" s="418"/>
-      <c r="D66" s="418"/>
-      <c r="E66" s="418"/>
-      <c r="F66" s="418"/>
-      <c r="G66" s="418"/>
-      <c r="H66" s="418"/>
-      <c r="I66" s="418"/>
-      <c r="J66" s="418"/>
-      <c r="K66" s="418"/>
-      <c r="L66" s="418"/>
-      <c r="M66" s="418"/>
-      <c r="N66" s="418"/>
-      <c r="O66" s="418"/>
-      <c r="P66" s="418"/>
-      <c r="Q66" s="418"/>
+      <c r="B66" s="409"/>
+      <c r="C66" s="409"/>
+      <c r="D66" s="409"/>
+      <c r="E66" s="409"/>
+      <c r="F66" s="409"/>
+      <c r="G66" s="409"/>
+      <c r="H66" s="409"/>
+      <c r="I66" s="409"/>
+      <c r="J66" s="409"/>
+      <c r="K66" s="409"/>
+      <c r="L66" s="409"/>
+      <c r="M66" s="409"/>
+      <c r="N66" s="409"/>
+      <c r="O66" s="409"/>
+      <c r="P66" s="409"/>
+      <c r="Q66" s="409"/>
       <c r="R66" s="6"/>
       <c r="S66" s="6"/>
       <c r="T66" s="114"/>
@@ -30715,23 +30715,23 @@
       <c r="AI66" s="115"/>
     </row>
     <row r="67" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="418"/>
-      <c r="B67" s="418"/>
-      <c r="C67" s="418"/>
-      <c r="D67" s="418"/>
-      <c r="E67" s="418"/>
-      <c r="F67" s="418"/>
-      <c r="G67" s="418"/>
-      <c r="H67" s="418"/>
-      <c r="I67" s="418"/>
-      <c r="J67" s="418"/>
-      <c r="K67" s="418"/>
-      <c r="L67" s="418"/>
-      <c r="M67" s="418"/>
-      <c r="N67" s="418"/>
-      <c r="O67" s="418"/>
-      <c r="P67" s="418"/>
-      <c r="Q67" s="418"/>
+      <c r="A67" s="409"/>
+      <c r="B67" s="409"/>
+      <c r="C67" s="409"/>
+      <c r="D67" s="409"/>
+      <c r="E67" s="409"/>
+      <c r="F67" s="409"/>
+      <c r="G67" s="409"/>
+      <c r="H67" s="409"/>
+      <c r="I67" s="409"/>
+      <c r="J67" s="409"/>
+      <c r="K67" s="409"/>
+      <c r="L67" s="409"/>
+      <c r="M67" s="409"/>
+      <c r="N67" s="409"/>
+      <c r="O67" s="409"/>
+      <c r="P67" s="409"/>
+      <c r="Q67" s="409"/>
       <c r="R67" s="6"/>
       <c r="S67" s="6"/>
       <c r="T67" s="114"/>
@@ -30752,25 +30752,25 @@
       <c r="AI67" s="115"/>
     </row>
     <row r="68" spans="1:35" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="417" t="s">
+      <c r="A68" s="406" t="s">
         <v>235</v>
       </c>
-      <c r="B68" s="417"/>
-      <c r="C68" s="417"/>
-      <c r="D68" s="417"/>
-      <c r="E68" s="417"/>
-      <c r="F68" s="417"/>
-      <c r="G68" s="417"/>
-      <c r="H68" s="417"/>
-      <c r="I68" s="417"/>
-      <c r="J68" s="417"/>
-      <c r="K68" s="417"/>
-      <c r="L68" s="417"/>
-      <c r="M68" s="417"/>
-      <c r="N68" s="417"/>
-      <c r="O68" s="417"/>
-      <c r="P68" s="417"/>
-      <c r="Q68" s="417"/>
+      <c r="B68" s="406"/>
+      <c r="C68" s="406"/>
+      <c r="D68" s="406"/>
+      <c r="E68" s="406"/>
+      <c r="F68" s="406"/>
+      <c r="G68" s="406"/>
+      <c r="H68" s="406"/>
+      <c r="I68" s="406"/>
+      <c r="J68" s="406"/>
+      <c r="K68" s="406"/>
+      <c r="L68" s="406"/>
+      <c r="M68" s="406"/>
+      <c r="N68" s="406"/>
+      <c r="O68" s="406"/>
+      <c r="P68" s="406"/>
+      <c r="Q68" s="406"/>
       <c r="R68" s="6"/>
       <c r="S68" s="6"/>
       <c r="T68" s="114"/>
@@ -30793,27 +30793,6 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="31">
-    <mergeCell ref="A68:Q68"/>
-    <mergeCell ref="A63:Q63"/>
-    <mergeCell ref="A64:Q64"/>
-    <mergeCell ref="A65:Q65"/>
-    <mergeCell ref="A66:Q66"/>
-    <mergeCell ref="A67:Q67"/>
-    <mergeCell ref="A58:Q58"/>
-    <mergeCell ref="A59:Q59"/>
-    <mergeCell ref="A60:Q60"/>
-    <mergeCell ref="A61:Q61"/>
-    <mergeCell ref="A62:Q62"/>
-    <mergeCell ref="A53:Q53"/>
-    <mergeCell ref="A54:Q54"/>
-    <mergeCell ref="A55:Q55"/>
-    <mergeCell ref="A56:Q56"/>
-    <mergeCell ref="A57:Q57"/>
-    <mergeCell ref="S4:Z4"/>
-    <mergeCell ref="AB4:AI4"/>
-    <mergeCell ref="A49:Q49"/>
-    <mergeCell ref="A51:Q51"/>
-    <mergeCell ref="A52:Q52"/>
     <mergeCell ref="A1:Q1"/>
     <mergeCell ref="B2:M2"/>
     <mergeCell ref="P2:Q3"/>
@@ -30824,6 +30803,27 @@
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="N3:O3"/>
+    <mergeCell ref="S4:Z4"/>
+    <mergeCell ref="AB4:AI4"/>
+    <mergeCell ref="A49:Q49"/>
+    <mergeCell ref="A51:Q51"/>
+    <mergeCell ref="A52:Q52"/>
+    <mergeCell ref="A53:Q53"/>
+    <mergeCell ref="A54:Q54"/>
+    <mergeCell ref="A55:Q55"/>
+    <mergeCell ref="A56:Q56"/>
+    <mergeCell ref="A57:Q57"/>
+    <mergeCell ref="A58:Q58"/>
+    <mergeCell ref="A59:Q59"/>
+    <mergeCell ref="A60:Q60"/>
+    <mergeCell ref="A61:Q61"/>
+    <mergeCell ref="A62:Q62"/>
+    <mergeCell ref="A68:Q68"/>
+    <mergeCell ref="A63:Q63"/>
+    <mergeCell ref="A64:Q64"/>
+    <mergeCell ref="A65:Q65"/>
+    <mergeCell ref="A66:Q66"/>
+    <mergeCell ref="A67:Q67"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A68" r:id="rId1"/>
@@ -30842,7 +30842,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
@@ -31797,13 +31797,13 @@
       <c r="R33" s="7"/>
     </row>
     <row r="34" spans="1:18" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="428" t="s">
+      <c r="A34" s="421" t="s">
         <v>247</v>
       </c>
-      <c r="B34" s="428"/>
-      <c r="C34" s="428"/>
-      <c r="D34" s="428"/>
-      <c r="E34" s="428"/>
+      <c r="B34" s="421"/>
+      <c r="C34" s="421"/>
+      <c r="D34" s="421"/>
+      <c r="E34" s="421"/>
       <c r="F34" s="6"/>
       <c r="G34" s="6"/>
       <c r="H34" s="6"/>
@@ -31852,13 +31852,13 @@
       <c r="R36" s="7"/>
     </row>
     <row r="37" spans="1:18" ht="139.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="431" t="s">
+      <c r="A37" s="419" t="s">
         <v>249</v>
       </c>
-      <c r="B37" s="431"/>
-      <c r="C37" s="431"/>
-      <c r="D37" s="431"/>
-      <c r="E37" s="431"/>
+      <c r="B37" s="419"/>
+      <c r="C37" s="419"/>
+      <c r="D37" s="419"/>
+      <c r="E37" s="419"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
       <c r="H37" s="6"/>
@@ -31874,13 +31874,13 @@
       <c r="R37" s="7"/>
     </row>
     <row r="38" spans="1:18" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="417" t="s">
+      <c r="A38" s="406" t="s">
         <v>250</v>
       </c>
-      <c r="B38" s="417"/>
-      <c r="C38" s="417"/>
-      <c r="D38" s="417"/>
-      <c r="E38" s="417"/>
+      <c r="B38" s="406"/>
+      <c r="C38" s="406"/>
+      <c r="D38" s="406"/>
+      <c r="E38" s="406"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
       <c r="H38" s="6"/>
@@ -32392,16 +32392,16 @@
       <c r="R16" s="7"/>
     </row>
     <row r="17" spans="1:18" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="428" t="s">
+      <c r="A17" s="421" t="s">
         <v>264</v>
       </c>
-      <c r="B17" s="428"/>
-      <c r="C17" s="428"/>
-      <c r="D17" s="428"/>
-      <c r="E17" s="428"/>
-      <c r="F17" s="428"/>
-      <c r="G17" s="428"/>
-      <c r="H17" s="428"/>
+      <c r="B17" s="421"/>
+      <c r="C17" s="421"/>
+      <c r="D17" s="421"/>
+      <c r="E17" s="421"/>
+      <c r="F17" s="421"/>
+      <c r="G17" s="421"/>
+      <c r="H17" s="421"/>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
@@ -32434,16 +32434,16 @@
       <c r="R18" s="7"/>
     </row>
     <row r="19" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="429" t="s">
+      <c r="A19" s="422" t="s">
         <v>265</v>
       </c>
-      <c r="B19" s="429"/>
-      <c r="C19" s="429"/>
-      <c r="D19" s="429"/>
-      <c r="E19" s="429"/>
-      <c r="F19" s="429"/>
-      <c r="G19" s="429"/>
-      <c r="H19" s="429"/>
+      <c r="B19" s="422"/>
+      <c r="C19" s="422"/>
+      <c r="D19" s="422"/>
+      <c r="E19" s="422"/>
+      <c r="F19" s="422"/>
+      <c r="G19" s="422"/>
+      <c r="H19" s="422"/>
       <c r="I19" s="76"/>
       <c r="J19" s="7"/>
       <c r="K19" s="7"/>
@@ -32456,16 +32456,16 @@
       <c r="R19" s="7"/>
     </row>
     <row r="20" spans="1:18" ht="93" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="431" t="s">
+      <c r="A20" s="419" t="s">
         <v>266</v>
       </c>
-      <c r="B20" s="431"/>
-      <c r="C20" s="431"/>
-      <c r="D20" s="431"/>
-      <c r="E20" s="431"/>
-      <c r="F20" s="431"/>
-      <c r="G20" s="431"/>
-      <c r="H20" s="431"/>
+      <c r="B20" s="419"/>
+      <c r="C20" s="419"/>
+      <c r="D20" s="419"/>
+      <c r="E20" s="419"/>
+      <c r="F20" s="419"/>
+      <c r="G20" s="419"/>
+      <c r="H20" s="419"/>
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
       <c r="K20" s="7"/>
@@ -32478,16 +32478,16 @@
       <c r="R20" s="7"/>
     </row>
     <row r="21" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="431" t="s">
+      <c r="A21" s="419" t="s">
         <v>267</v>
       </c>
-      <c r="B21" s="431"/>
-      <c r="C21" s="431"/>
-      <c r="D21" s="431"/>
-      <c r="E21" s="431"/>
-      <c r="F21" s="431"/>
-      <c r="G21" s="431"/>
-      <c r="H21" s="431"/>
+      <c r="B21" s="419"/>
+      <c r="C21" s="419"/>
+      <c r="D21" s="419"/>
+      <c r="E21" s="419"/>
+      <c r="F21" s="419"/>
+      <c r="G21" s="419"/>
+      <c r="H21" s="419"/>
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
       <c r="K21" s="7"/>
@@ -32500,16 +32500,16 @@
       <c r="R21" s="7"/>
     </row>
     <row r="22" spans="1:18" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="431" t="s">
+      <c r="A22" s="419" t="s">
         <v>268</v>
       </c>
-      <c r="B22" s="431"/>
-      <c r="C22" s="431"/>
-      <c r="D22" s="431"/>
-      <c r="E22" s="431"/>
-      <c r="F22" s="431"/>
-      <c r="G22" s="431"/>
-      <c r="H22" s="431"/>
+      <c r="B22" s="419"/>
+      <c r="C22" s="419"/>
+      <c r="D22" s="419"/>
+      <c r="E22" s="419"/>
+      <c r="F22" s="419"/>
+      <c r="G22" s="419"/>
+      <c r="H22" s="419"/>
       <c r="I22" s="76"/>
       <c r="J22" s="7"/>
       <c r="K22" s="7"/>
@@ -32522,16 +32522,16 @@
       <c r="R22" s="7"/>
     </row>
     <row r="23" spans="1:18" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="431" t="s">
+      <c r="A23" s="419" t="s">
         <v>269</v>
       </c>
-      <c r="B23" s="431"/>
-      <c r="C23" s="431"/>
-      <c r="D23" s="431"/>
-      <c r="E23" s="431"/>
-      <c r="F23" s="431"/>
-      <c r="G23" s="431"/>
-      <c r="H23" s="431"/>
+      <c r="B23" s="419"/>
+      <c r="C23" s="419"/>
+      <c r="D23" s="419"/>
+      <c r="E23" s="419"/>
+      <c r="F23" s="419"/>
+      <c r="G23" s="419"/>
+      <c r="H23" s="419"/>
       <c r="I23" s="7"/>
       <c r="J23" s="7"/>
       <c r="K23" s="7"/>
@@ -32544,16 +32544,16 @@
       <c r="R23" s="7"/>
     </row>
     <row r="24" spans="1:18" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="413" t="s">
+      <c r="A24" s="410" t="s">
         <v>270</v>
       </c>
-      <c r="B24" s="413"/>
-      <c r="C24" s="413"/>
-      <c r="D24" s="413"/>
-      <c r="E24" s="413"/>
-      <c r="F24" s="413"/>
-      <c r="G24" s="413"/>
-      <c r="H24" s="413"/>
+      <c r="B24" s="410"/>
+      <c r="C24" s="410"/>
+      <c r="D24" s="410"/>
+      <c r="E24" s="410"/>
+      <c r="F24" s="410"/>
+      <c r="G24" s="410"/>
+      <c r="H24" s="410"/>
       <c r="I24" s="76"/>
       <c r="J24" s="7"/>
       <c r="K24" s="7"/>
@@ -32566,16 +32566,16 @@
       <c r="R24" s="7"/>
     </row>
     <row r="25" spans="1:18" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="431" t="s">
+      <c r="A25" s="419" t="s">
         <v>271</v>
       </c>
-      <c r="B25" s="431"/>
-      <c r="C25" s="431"/>
-      <c r="D25" s="431"/>
-      <c r="E25" s="431"/>
-      <c r="F25" s="431"/>
-      <c r="G25" s="431"/>
-      <c r="H25" s="431"/>
+      <c r="B25" s="419"/>
+      <c r="C25" s="419"/>
+      <c r="D25" s="419"/>
+      <c r="E25" s="419"/>
+      <c r="F25" s="419"/>
+      <c r="G25" s="419"/>
+      <c r="H25" s="419"/>
       <c r="I25" s="7"/>
       <c r="J25" s="7"/>
       <c r="K25" s="7"/>
@@ -32588,16 +32588,16 @@
       <c r="R25" s="7"/>
     </row>
     <row r="26" spans="1:18" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="431" t="s">
+      <c r="A26" s="419" t="s">
         <v>272</v>
       </c>
-      <c r="B26" s="431"/>
-      <c r="C26" s="431"/>
-      <c r="D26" s="431"/>
-      <c r="E26" s="431"/>
-      <c r="F26" s="431"/>
-      <c r="G26" s="431"/>
-      <c r="H26" s="431"/>
+      <c r="B26" s="419"/>
+      <c r="C26" s="419"/>
+      <c r="D26" s="419"/>
+      <c r="E26" s="419"/>
+      <c r="F26" s="419"/>
+      <c r="G26" s="419"/>
+      <c r="H26" s="419"/>
       <c r="I26" s="76"/>
       <c r="J26" s="7"/>
       <c r="K26" s="7"/>
@@ -32610,16 +32610,16 @@
       <c r="R26" s="7"/>
     </row>
     <row r="27" spans="1:18" ht="63" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="431" t="s">
+      <c r="A27" s="419" t="s">
         <v>273</v>
       </c>
-      <c r="B27" s="431"/>
-      <c r="C27" s="431"/>
-      <c r="D27" s="431"/>
-      <c r="E27" s="431"/>
-      <c r="F27" s="431"/>
-      <c r="G27" s="431"/>
-      <c r="H27" s="431"/>
+      <c r="B27" s="419"/>
+      <c r="C27" s="419"/>
+      <c r="D27" s="419"/>
+      <c r="E27" s="419"/>
+      <c r="F27" s="419"/>
+      <c r="G27" s="419"/>
+      <c r="H27" s="419"/>
       <c r="I27" s="7"/>
       <c r="J27" s="7"/>
       <c r="K27" s="7"/>
@@ -32632,16 +32632,16 @@
       <c r="R27" s="7"/>
     </row>
     <row r="28" spans="1:18" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="431" t="s">
+      <c r="A28" s="419" t="s">
         <v>274</v>
       </c>
-      <c r="B28" s="431"/>
-      <c r="C28" s="431"/>
-      <c r="D28" s="431"/>
-      <c r="E28" s="431"/>
-      <c r="F28" s="431"/>
-      <c r="G28" s="431"/>
-      <c r="H28" s="431"/>
+      <c r="B28" s="419"/>
+      <c r="C28" s="419"/>
+      <c r="D28" s="419"/>
+      <c r="E28" s="419"/>
+      <c r="F28" s="419"/>
+      <c r="G28" s="419"/>
+      <c r="H28" s="419"/>
       <c r="I28" s="76"/>
       <c r="J28" s="7"/>
       <c r="K28" s="7"/>
@@ -32654,16 +32654,16 @@
       <c r="R28" s="7"/>
     </row>
     <row r="29" spans="1:18" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="417" t="s">
+      <c r="A29" s="406" t="s">
         <v>275</v>
       </c>
-      <c r="B29" s="417"/>
-      <c r="C29" s="417"/>
-      <c r="D29" s="417"/>
-      <c r="E29" s="417"/>
-      <c r="F29" s="417"/>
-      <c r="G29" s="417"/>
-      <c r="H29" s="417"/>
+      <c r="B29" s="406"/>
+      <c r="C29" s="406"/>
+      <c r="D29" s="406"/>
+      <c r="E29" s="406"/>
+      <c r="F29" s="406"/>
+      <c r="G29" s="406"/>
+      <c r="H29" s="406"/>
       <c r="I29" s="7"/>
       <c r="J29" s="7"/>
       <c r="K29" s="7"/>
@@ -32758,21 +32758,21 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="15">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="A20:H20"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="A22:H22"/>
+    <mergeCell ref="A23:H23"/>
+    <mergeCell ref="A24:H24"/>
     <mergeCell ref="A25:H25"/>
     <mergeCell ref="A26:H26"/>
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="A28:H28"/>
     <mergeCell ref="A29:H29"/>
-    <mergeCell ref="A20:H20"/>
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="A22:H22"/>
-    <mergeCell ref="A23:H23"/>
-    <mergeCell ref="A24:H24"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A17:H17"/>
-    <mergeCell ref="A19:H19"/>
   </mergeCells>
   <dataValidations count="8">
     <dataValidation type="whole" error="Please check this salary information as it is outside the normal range._x000a_" sqref="B7">
@@ -33247,16 +33247,16 @@
       <c r="R12" s="6"/>
     </row>
     <row r="13" spans="1:21" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="428" t="s">
+      <c r="A13" s="421" t="s">
         <v>284</v>
       </c>
-      <c r="B13" s="428"/>
-      <c r="C13" s="428"/>
-      <c r="D13" s="428"/>
-      <c r="E13" s="428"/>
-      <c r="F13" s="428"/>
-      <c r="G13" s="428"/>
-      <c r="H13" s="428"/>
+      <c r="B13" s="421"/>
+      <c r="C13" s="421"/>
+      <c r="D13" s="421"/>
+      <c r="E13" s="421"/>
+      <c r="F13" s="421"/>
+      <c r="G13" s="421"/>
+      <c r="H13" s="421"/>
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
@@ -33289,15 +33289,15 @@
       <c r="R14" s="14"/>
     </row>
     <row r="15" spans="1:21" ht="107.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="430" t="s">
+      <c r="A15" s="423" t="s">
         <v>285</v>
       </c>
-      <c r="B15" s="430"/>
-      <c r="C15" s="430"/>
-      <c r="D15" s="430"/>
-      <c r="E15" s="430"/>
-      <c r="F15" s="430"/>
-      <c r="G15" s="430"/>
+      <c r="B15" s="423"/>
+      <c r="C15" s="423"/>
+      <c r="D15" s="423"/>
+      <c r="E15" s="423"/>
+      <c r="F15" s="423"/>
+      <c r="G15" s="423"/>
       <c r="H15" s="16"/>
       <c r="I15" s="16"/>
       <c r="J15" s="16"/>

</xml_diff>